<commit_message>
Added ARPPU and user growth
</commit_message>
<xml_diff>
--- a/BMBL.xlsx
+++ b/BMBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Development\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517ED249-862C-4883-A3C9-5308CF4A38D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC82A1EA-8F4F-47E7-A2A3-5E7D3B882624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="31845" windowHeight="20985" tabRatio="946" activeTab="3" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3208" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3214" uniqueCount="581">
   <si>
     <r>
       <t xml:space="preserve">This Excel file is intended </t>
@@ -1843,9 +1843,6 @@
     <t>Cash</t>
   </si>
   <si>
-    <t>Bumble revenue per paying user ($)</t>
-  </si>
-  <si>
     <t>$mn</t>
   </si>
   <si>
@@ -1861,16 +1858,37 @@
     <t>Total paying users (mn)</t>
   </si>
   <si>
-    <t>Badoo and other revenue per paying user ($)</t>
-  </si>
-  <si>
-    <t>Total average rev. per paying user ($)</t>
-  </si>
-  <si>
     <t>Bumble</t>
   </si>
   <si>
     <t>Badoo and other</t>
+  </si>
+  <si>
+    <t>Bumble paying user growth</t>
+  </si>
+  <si>
+    <t>Badoo paying user growth</t>
+  </si>
+  <si>
+    <t>Total paying user growth</t>
+  </si>
+  <si>
+    <t>Bumble ARPPU ($)</t>
+  </si>
+  <si>
+    <t>Badoo and other ARPPU ($)</t>
+  </si>
+  <si>
+    <t>Total ARRPU ($)</t>
+  </si>
+  <si>
+    <t>Bumble ARPPU growth</t>
+  </si>
+  <si>
+    <t>Badoo ARPPU growth</t>
+  </si>
+  <si>
+    <t>Total ARPPU growth</t>
   </si>
 </sst>
 </file>
@@ -2081,7 +2099,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2199,6 +2217,9 @@
     </xf>
     <xf numFmtId="170" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2260,16 +2281,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>571244</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>21290</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>371219</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>145115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>554972</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>47063</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>354947</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>28013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2293,7 +2314,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15677894" y="4840940"/>
+          <a:off x="17744819" y="6279215"/>
           <a:ext cx="7070328" cy="2673723"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2305,16 +2326,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>414619</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>153441</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>27216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>525001</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>143617</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>239250</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>116404</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2337,8 +2358,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20836219" y="10201274"/>
-          <a:ext cx="4244232" cy="2801093"/>
+          <a:off x="21543870" y="11198680"/>
+          <a:ext cx="4766666" cy="3205224"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7546,7 +7567,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -17283,10 +17304,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:AO743"/>
+  <dimension ref="A1:AG750"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X47" sqref="X47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -17554,7 +17575,7 @@
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
       <c r="E11" s="60" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F11" s="61">
         <v>694.32899999999995</v>
@@ -17625,7 +17646,7 @@
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
       <c r="E12" s="60" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="F12" s="61">
         <v>209.17400000000001</v>
@@ -17834,7 +17855,7 @@
         <v>-64.581000000000003</v>
       </c>
       <c r="O14" s="39">
-        <f t="shared" ref="O13:O18" ca="1" si="4">F14-SUM(L14:N14)</f>
+        <f t="shared" ref="O14:O18" ca="1" si="4">F14-SUM(L14:N14)</f>
         <v>-65.371000000000009</v>
       </c>
       <c r="P14" s="39">
@@ -17850,7 +17871,7 @@
         <v>-80.049000000000007</v>
       </c>
       <c r="S14" s="39">
-        <f t="shared" ref="S13:S18" ca="1" si="5">G14-SUM(P14:R14)</f>
+        <f t="shared" ref="S14:S18" ca="1" si="5">G14-SUM(P14:R14)</f>
         <v>-80.468999999999966</v>
       </c>
       <c r="T14" s="39">
@@ -17866,7 +17887,7 @@
         <v>-79.552000000000007</v>
       </c>
       <c r="W14" s="39">
-        <f t="shared" ref="W13:W27" ca="1" si="6">H14-SUM(T14:V14)</f>
+        <f t="shared" ref="W14:W27" ca="1" si="6">H14-SUM(T14:V14)</f>
         <v>-77.952999999999975</v>
       </c>
       <c r="X14" s="39">
@@ -19399,23 +19420,23 @@
       <c r="AF32" s="40"/>
       <c r="AG32" s="40"/>
     </row>
-    <row r="33" spans="1:41" ht="3" customHeight="1"/>
-    <row r="34" spans="1:41">
+    <row r="33" spans="1:26" ht="3" customHeight="1"/>
+    <row r="34" spans="1:26">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="E34" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="W34" s="58"/>
     </row>
-    <row r="35" spans="1:41">
+    <row r="35" spans="1:26">
       <c r="A35" s="33"/>
       <c r="B35" s="33"/>
       <c r="E35" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F35" s="52">
         <v>2.0022000000000002</v>
@@ -19426,8 +19447,8 @@
       <c r="H35" s="52">
         <v>2.8073000000000001</v>
       </c>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
       <c r="L35" s="52">
         <v>1.7751999999999999</v>
       </c>
@@ -19471,12 +19492,13 @@
         <v>2.7084000000000001</v>
       </c>
       <c r="Y35" s="12"/>
-    </row>
-    <row r="36" spans="1:41">
+      <c r="Z35" s="39"/>
+    </row>
+    <row r="36" spans="1:26">
       <c r="A36" s="33"/>
       <c r="B36" s="33"/>
       <c r="E36" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F36" s="52">
         <v>1.1797</v>
@@ -19487,8 +19509,8 @@
       <c r="H36" s="52">
         <v>1.3420000000000001</v>
       </c>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
       <c r="L36" s="52">
         <v>1.232</v>
       </c>
@@ -19532,12 +19554,13 @@
         <v>1.3063</v>
       </c>
       <c r="Y36" s="12"/>
-    </row>
-    <row r="37" spans="1:41">
+      <c r="Z36" s="39"/>
+    </row>
+    <row r="37" spans="1:26">
       <c r="A37" s="33"/>
       <c r="B37" s="33"/>
       <c r="E37" s="45" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F37" s="46">
         <f t="shared" ref="F37:H37" si="32">SUM(F35:F36)</f>
@@ -19551,8 +19574,8 @@
         <f t="shared" si="32"/>
         <v>4.1493000000000002</v>
       </c>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
       <c r="L37" s="46">
         <f t="shared" ref="L37:W37" si="33">SUM(L35:L36)</f>
         <v>3.0072000000000001</v>
@@ -19606,15 +19629,16 @@
         <v>4.0147000000000004</v>
       </c>
       <c r="Y37" s="12"/>
-    </row>
-    <row r="38" spans="1:41" ht="1.5" customHeight="1">
+      <c r="Z37" s="39"/>
+    </row>
+    <row r="38" spans="1:26" ht="1.5" customHeight="1">
       <c r="A38" s="33"/>
       <c r="B38" s="33"/>
       <c r="F38" s="57"/>
       <c r="G38" s="57"/>
       <c r="H38" s="57"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
@@ -19630,11 +19654,11 @@
       <c r="X38" s="12"/>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="1:41">
+    <row r="39" spans="1:26">
       <c r="A39" s="33"/>
       <c r="B39" s="33"/>
       <c r="E39" s="3" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="F39" s="52">
         <v>28.9</v>
@@ -19645,8 +19669,8 @@
       <c r="H39" s="52">
         <v>25.72</v>
       </c>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
       <c r="L39" s="52">
         <v>28.99</v>
       </c>
@@ -19691,11 +19715,11 @@
       </c>
       <c r="Y39" s="52"/>
     </row>
-    <row r="40" spans="1:41">
+    <row r="40" spans="1:26">
       <c r="A40" s="33"/>
       <c r="B40" s="33"/>
       <c r="E40" s="3" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="F40" s="52">
         <v>13.06</v>
@@ -19706,8 +19730,8 @@
       <c r="H40" s="52">
         <v>11.85</v>
       </c>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
       <c r="L40" s="52">
         <v>13.48</v>
       </c>
@@ -19752,11 +19776,11 @@
       </c>
       <c r="Y40" s="52"/>
     </row>
-    <row r="41" spans="1:41">
+    <row r="41" spans="1:26">
       <c r="A41" s="33"/>
       <c r="B41" s="33"/>
       <c r="E41" s="45" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="F41" s="46">
         <f t="shared" ref="F41:H41" si="34">F35/F37*F39+F36/F37*F40</f>
@@ -19770,8 +19794,8 @@
         <f t="shared" si="34"/>
         <v>21.23405297279059</v>
       </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
       <c r="L41" s="46">
         <f t="shared" ref="L41:W41" si="35">L35/L37*L39+L36/L37*L40</f>
         <v>22.635810055865921</v>
@@ -19826,7 +19850,7 @@
       </c>
       <c r="Y41" s="12"/>
     </row>
-    <row r="42" spans="1:41">
+    <row r="42" spans="1:26">
       <c r="A42" s="33"/>
       <c r="B42" s="33"/>
       <c r="F42" s="12"/>
@@ -19849,185 +19873,232 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
     </row>
-    <row r="43" spans="1:41">
+    <row r="43" spans="1:26">
       <c r="A43" s="33"/>
       <c r="B43" s="33"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="12"/>
-      <c r="Q43" s="12"/>
-      <c r="R43" s="12"/>
-      <c r="S43" s="12"/>
-      <c r="T43" s="12"/>
-      <c r="U43" s="12"/>
-      <c r="V43" s="12"/>
-      <c r="W43" s="12"/>
-      <c r="X43" s="12"/>
+      <c r="E43" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="F43" s="15" t="str">
+        <f t="shared" ref="F43:H45" si="36">IFERROR(+F35/E35-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="G43" s="15">
+        <f t="shared" si="36"/>
+        <v>0.25731695135351096</v>
+      </c>
+      <c r="H43" s="15">
+        <f t="shared" si="36"/>
+        <v>0.11515849686184176</v>
+      </c>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="L43" s="15" t="str">
+        <f t="shared" ref="L43" si="37">IFERROR(+L35/K35-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="M43" s="15">
+        <f t="shared" ref="M43:W49" si="38">IFERROR(+M35/L35-1,"n/a")</f>
+        <v>8.4103199639477433E-2</v>
+      </c>
+      <c r="N43" s="15">
+        <f t="shared" si="38"/>
+        <v>8.5009093270979275E-2</v>
+      </c>
+      <c r="O43" s="15">
+        <f t="shared" si="38"/>
+        <v>6.3646377089220385E-2</v>
+      </c>
+      <c r="P43" s="15">
+        <f t="shared" si="38"/>
+        <v>4.4034218820350635E-2</v>
+      </c>
+      <c r="Q43" s="15">
+        <f t="shared" si="38"/>
+        <v>5.9944799033983198E-2</v>
+      </c>
+      <c r="R43" s="15">
+        <f t="shared" si="38"/>
+        <v>5.9850272601513543E-2</v>
+      </c>
+      <c r="S43" s="15">
+        <f t="shared" si="38"/>
+        <v>3.1939805750699879E-2</v>
+      </c>
+      <c r="T43" s="15">
+        <f t="shared" si="38"/>
+        <v>1.5587217737436099E-2</v>
+      </c>
+      <c r="U43" s="15">
+        <f t="shared" si="38"/>
+        <v>3.1941391941392006E-2</v>
+      </c>
+      <c r="V43" s="15">
+        <f t="shared" si="38"/>
+        <v>1.8493539684793392E-2</v>
+      </c>
+      <c r="W43" s="15">
+        <f t="shared" si="38"/>
+        <v>-1.9726065590910724E-2</v>
+      </c>
+      <c r="X43" s="15">
+        <f>IFERROR(+X35/W35-1,"n/a")</f>
+        <v>-3.7081807515909948E-2</v>
+      </c>
       <c r="Y43" s="12"/>
     </row>
-    <row r="44" spans="1:41">
-      <c r="A44" s="33" t="s">
-        <v>547</v>
-      </c>
+    <row r="44" spans="1:26">
+      <c r="A44" s="33"/>
       <c r="B44" s="33"/>
-      <c r="E44" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'is_fy" &amp; F$2 &amp; F$1 &amp; "'!E:E"), INDIRECT("'is_fy" &amp; F$2 &amp; F$1 &amp; "'!A:A"), $A44) / $B$3</f>
-        <v>-79.745999999999995</v>
-      </c>
-      <c r="G44" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'is_fy" &amp; G$2 &amp; G$1 &amp; "'!E:E"), INDIRECT("'is_fy" &amp; G$2 &amp; G$1 &amp; "'!A:A"), $A44) / $B$3</f>
-        <v>-4.2130000000000001</v>
-      </c>
-      <c r="H44" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'is_fy" &amp; H$2 &amp; H$1 &amp; "'!E:E"), INDIRECT("'is_fy" &amp; H$2 &amp; H$1 &amp; "'!A:A"), $A44) / $B$3</f>
-        <v>-557.00800000000004</v>
-      </c>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="L44" s="62">
-        <f t="shared" ref="L44:V44" ca="1" si="36">SUMIFS(INDIRECT("'is_q" &amp; L$2 &amp; L$1 &amp; "'!E:E"), INDIRECT("'is_q" &amp; L$2 &amp; L$1 &amp; "'!A:A"), $A44) / $B$3</f>
-        <v>16.395</v>
-      </c>
-      <c r="M44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>-4.3920000000000003</v>
-      </c>
-      <c r="N44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>18.062999999999999</v>
-      </c>
-      <c r="O44" s="62"/>
-      <c r="P44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>-1.611</v>
-      </c>
-      <c r="Q44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>6.7530000000000001</v>
-      </c>
-      <c r="R44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>16.670999999999999</v>
-      </c>
-      <c r="S44" s="62"/>
-      <c r="T44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>24.617000000000001</v>
-      </c>
-      <c r="U44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>27.395</v>
-      </c>
-      <c r="V44" s="62">
-        <f t="shared" ca="1" si="36"/>
-        <v>-613.19899999999996</v>
-      </c>
-      <c r="W44" s="62"/>
-      <c r="X44" s="62">
-        <f ca="1">SUMIFS(INDIRECT("'is_q" &amp; X$2 &amp; X$1 &amp; "'!E:E"), INDIRECT("'is_q" &amp; X$2 &amp; X$1 &amp; "'!A:A"), $A44) / $B$3</f>
-        <v>13.444000000000001</v>
-      </c>
-      <c r="AN44">
-        <v>244</v>
-      </c>
-      <c r="AO44">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="45" spans="1:41">
+      <c r="E44" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="F44" s="15" t="str">
+        <f t="shared" si="36"/>
+        <v>n/a</v>
+      </c>
+      <c r="G44" s="15">
+        <f t="shared" si="36"/>
+        <v>2.000508603882345E-2</v>
+      </c>
+      <c r="H44" s="15">
+        <f t="shared" si="36"/>
+        <v>0.11526635086844506</v>
+      </c>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="L44" s="15" t="str">
+        <f t="shared" ref="L44" si="39">IFERROR(+L36/K36-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="M44" s="15">
+        <f t="shared" si="38"/>
+        <v>-0.11022727272727262</v>
+      </c>
+      <c r="N44" s="15">
+        <f t="shared" si="38"/>
+        <v>9.6697682904579363E-2</v>
+      </c>
+      <c r="O44" s="15">
+        <f t="shared" si="38"/>
+        <v>-1.1478955248710676E-2</v>
+      </c>
+      <c r="P44" s="15">
+        <f t="shared" si="38"/>
+        <v>-3.9885560417367794E-2</v>
+      </c>
+      <c r="Q44" s="15">
+        <f t="shared" si="38"/>
+        <v>3.0236634531113138E-2</v>
+      </c>
+      <c r="R44" s="15">
+        <f t="shared" si="38"/>
+        <v>3.4113143343258212E-2</v>
+      </c>
+      <c r="S44" s="15">
+        <f t="shared" si="38"/>
+        <v>5.388285620269806E-2</v>
+      </c>
+      <c r="T44" s="15">
+        <f t="shared" si="38"/>
+        <v>1.03036453048162E-2</v>
+      </c>
+      <c r="U44" s="15">
+        <f t="shared" si="38"/>
+        <v>2.0937958742177187E-2</v>
+      </c>
+      <c r="V44" s="15">
+        <f t="shared" si="38"/>
+        <v>4.9038898138338283E-2</v>
+      </c>
+      <c r="W44" s="15">
+        <f t="shared" si="38"/>
+        <v>-1.4500072139662423E-2</v>
+      </c>
+      <c r="X44" s="15">
+        <f>IFERROR(+X36/W36-1,"n/a")</f>
+        <v>-4.3774247858868409E-2</v>
+      </c>
+      <c r="Y44" s="12"/>
+    </row>
+    <row r="45" spans="1:26">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
-      <c r="C45" s="11" t="b" cm="1">
-        <f t="array" aca="1" ref="C45" ca="1">AND(F45:AC45&lt;$B$1,F45:AC45&gt;-$B$1)</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" s="13">
-        <f ca="1">+F44-F27</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="13">
-        <f ca="1">+G44-G27</f>
-        <v>1.1457501614131615E-13</v>
-      </c>
-      <c r="H45" s="13">
-        <f ca="1">+H44-H27</f>
-        <v>0</v>
-      </c>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="L45" s="34">
-        <f ca="1">+L44-L27</f>
-        <v>1.1690000000000396</v>
-      </c>
-      <c r="M45" s="34">
-        <f ca="1">+M44-M27</f>
-        <v>1.248000000000018</v>
-      </c>
-      <c r="N45" s="34">
-        <f ca="1">+N44-N27</f>
-        <v>0</v>
-      </c>
-      <c r="O45" s="34">
-        <f ca="1">F27-SUM(L27:O27)</f>
-        <v>0</v>
-      </c>
-      <c r="P45" s="34">
-        <f ca="1">+P44-P27</f>
-        <v>1.4432899320127035E-14</v>
-      </c>
-      <c r="Q45" s="34">
-        <f ca="1">+Q44-Q27</f>
-        <v>-2.6645352591003757E-14</v>
-      </c>
-      <c r="R45" s="34">
-        <f ca="1">+R44-R27</f>
-        <v>0</v>
-      </c>
-      <c r="S45" s="34">
-        <f ca="1">G27-SUM(P27:S27)</f>
-        <v>-2.0605739337042905E-13</v>
-      </c>
-      <c r="T45" s="34">
-        <f ca="1">+T44-T27</f>
-        <v>0</v>
-      </c>
-      <c r="U45" s="34">
-        <f ca="1">+U44-U27</f>
-        <v>0</v>
-      </c>
-      <c r="V45" s="34">
-        <f ca="1">+V44-V27</f>
-        <v>0</v>
-      </c>
-      <c r="W45" s="34">
-        <f ca="1">H27-SUM(T27:W27)</f>
-        <v>0</v>
-      </c>
-      <c r="X45" s="34">
-        <f ca="1">+X44-X27</f>
-        <v>2.3092638912203256E-14</v>
-      </c>
-      <c r="AO45">
-        <f>AO44+AN44</f>
-        <v>493</v>
-      </c>
-    </row>
-    <row r="46" spans="1:41">
+      <c r="E45" s="45" t="s">
+        <v>574</v>
+      </c>
+      <c r="F45" s="63" t="str">
+        <f t="shared" si="36"/>
+        <v>n/a</v>
+      </c>
+      <c r="G45" s="63">
+        <f t="shared" si="36"/>
+        <v>0.16933278858543632</v>
+      </c>
+      <c r="H45" s="63">
+        <f t="shared" si="36"/>
+        <v>0.11519337759023851</v>
+      </c>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="L45" s="63" t="str">
+        <f t="shared" ref="L45" si="40">IFERROR(+L37/K37-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="M45" s="63">
+        <f t="shared" si="38"/>
+        <v>4.4892258579409816E-3</v>
+      </c>
+      <c r="N45" s="63">
+        <f t="shared" si="38"/>
+        <v>8.9250835898963654E-2</v>
+      </c>
+      <c r="O45" s="63">
+        <f t="shared" si="38"/>
+        <v>3.619730723642256E-2</v>
+      </c>
+      <c r="P45" s="63">
+        <f t="shared" si="38"/>
+        <v>1.4782659705519841E-2</v>
+      </c>
+      <c r="Q45" s="63">
+        <f t="shared" si="38"/>
+        <v>5.014740736458756E-2</v>
+      </c>
+      <c r="R45" s="63">
+        <f t="shared" si="38"/>
+        <v>5.1523408471637389E-2</v>
+      </c>
+      <c r="S45" s="63">
+        <f t="shared" si="38"/>
+        <v>3.8921607119486445E-2</v>
+      </c>
+      <c r="T45" s="63">
+        <f t="shared" si="38"/>
+        <v>1.3881890557291721E-2</v>
+      </c>
+      <c r="U45" s="63">
+        <f t="shared" si="38"/>
+        <v>2.8402455085356548E-2</v>
+      </c>
+      <c r="V45" s="63">
+        <f t="shared" si="38"/>
+        <v>2.824626685352527E-2</v>
+      </c>
+      <c r="W45" s="63">
+        <f t="shared" si="38"/>
+        <v>-1.8023733991305302E-2</v>
+      </c>
+      <c r="X45" s="63">
+        <f>IFERROR(+X37/W37-1,"n/a")</f>
+        <v>-3.9269646788551604E-2</v>
+      </c>
+      <c r="Y45" s="12"/>
+    </row>
+    <row r="46" spans="1:26">
       <c r="A46" s="33"/>
       <c r="B46" s="33"/>
+      <c r="E46" s="3"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -20047,1384 +20118,1616 @@
       <c r="W46" s="12"/>
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
-      <c r="AO46">
-        <f>+AO45/2</f>
-        <v>246.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:41">
+    </row>
+    <row r="47" spans="1:26">
       <c r="A47" s="33"/>
       <c r="B47" s="33"/>
-      <c r="E47" s="2" t="str">
+      <c r="E47" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="F47" s="15" t="str">
+        <f t="shared" ref="F47:F49" si="41">IFERROR(+F39/E39-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="G47" s="15">
+        <f t="shared" ref="G47:G49" si="42">IFERROR(+G39/F39-1,"n/a")</f>
+        <v>-3.2179930795847689E-2</v>
+      </c>
+      <c r="H47" s="15">
+        <f t="shared" ref="H47:H49" si="43">IFERROR(+H39/G39-1,"n/a")</f>
+        <v>-8.0443332141580282E-2</v>
+      </c>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="L47" s="15" t="str">
+        <f t="shared" ref="L47:L49" si="44">IFERROR(+L39/K39-1,"n/a")</f>
+        <v>n/a</v>
+      </c>
+      <c r="M47" s="15">
+        <f t="shared" si="38"/>
+        <v>6.553984132459556E-3</v>
+      </c>
+      <c r="N47" s="15">
+        <f t="shared" si="38"/>
+        <v>-1.1651816312542862E-2</v>
+      </c>
+      <c r="O47" s="15">
+        <f t="shared" si="38"/>
+        <v>-6.8376025676818442E-3</v>
+      </c>
+      <c r="P47" s="15">
+        <f t="shared" si="38"/>
+        <v>-2.48859557656127E-2</v>
+      </c>
+      <c r="Q47" s="15">
+        <f t="shared" si="38"/>
+        <v>1.0025062656641603E-2</v>
+      </c>
+      <c r="R47" s="15">
+        <f t="shared" si="38"/>
+        <v>6.0262318326833597E-3</v>
+      </c>
+      <c r="S47" s="15">
+        <f t="shared" si="38"/>
+        <v>-3.5522425432995219E-2</v>
+      </c>
+      <c r="T47" s="15">
+        <f t="shared" si="38"/>
+        <v>-3.7698316986432334E-2</v>
+      </c>
+      <c r="U47" s="15">
+        <f t="shared" si="38"/>
+        <v>-2.0880789673500377E-2</v>
+      </c>
+      <c r="V47" s="15">
+        <f t="shared" si="38"/>
+        <v>-8.1426909654905844E-3</v>
+      </c>
+      <c r="W47" s="15">
+        <f t="shared" si="38"/>
+        <v>-1.6153129270075284E-2</v>
+      </c>
+      <c r="X47" s="15">
+        <f>IFERROR(+X39/W39-1,"n/a")</f>
+        <v>-1.2985477491052944E-2</v>
+      </c>
+      <c r="Y47" s="12"/>
+    </row>
+    <row r="48" spans="1:26">
+      <c r="A48" s="33"/>
+      <c r="B48" s="33"/>
+      <c r="E48" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="F48" s="15" t="str">
+        <f t="shared" si="41"/>
+        <v>n/a</v>
+      </c>
+      <c r="G48" s="15">
+        <f t="shared" si="42"/>
+        <v>-2.7565084226646386E-2</v>
+      </c>
+      <c r="H48" s="15">
+        <f t="shared" si="43"/>
+        <v>-6.6929133858267709E-2</v>
+      </c>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="L48" s="15" t="str">
+        <f t="shared" si="44"/>
+        <v>n/a</v>
+      </c>
+      <c r="M48" s="15">
+        <f t="shared" si="38"/>
+        <v>5.9347181008901906E-3</v>
+      </c>
+      <c r="N48" s="15">
+        <f t="shared" si="38"/>
+        <v>-5.9734513274336321E-2</v>
+      </c>
+      <c r="O48" s="15">
+        <f t="shared" si="38"/>
+        <v>0.1171388784392926</v>
+      </c>
+      <c r="P48" s="15">
+        <f t="shared" si="38"/>
+        <v>-0.12451420806994762</v>
+      </c>
+      <c r="Q48" s="15">
+        <f t="shared" si="38"/>
+        <v>2.8869286287088958E-2</v>
+      </c>
+      <c r="R48" s="15">
+        <f t="shared" si="38"/>
+        <v>-3.1176929072487258E-3</v>
+      </c>
+      <c r="S48" s="15">
+        <f t="shared" si="38"/>
+        <v>7.6210588913737443E-2</v>
+      </c>
+      <c r="T48" s="15">
+        <f t="shared" si="38"/>
+        <v>-0.10277957355109479</v>
+      </c>
+      <c r="U48" s="15">
+        <f t="shared" si="38"/>
+        <v>-3.4008097165991846E-2</v>
+      </c>
+      <c r="V48" s="15">
+        <f t="shared" si="38"/>
+        <v>8.3822296730931001E-3</v>
+      </c>
+      <c r="W48" s="15">
+        <f t="shared" si="38"/>
+        <v>-2.9509630424973121E-4</v>
+      </c>
+      <c r="X48" s="15">
+        <f>IFERROR(+X40/W40-1,"n/a")</f>
+        <v>-0.10863139100795338</v>
+      </c>
+      <c r="Y48" s="12"/>
+    </row>
+    <row r="49" spans="1:25">
+      <c r="A49" s="33"/>
+      <c r="B49" s="33"/>
+      <c r="E49" s="45" t="s">
+        <v>580</v>
+      </c>
+      <c r="F49" s="63" t="str">
+        <f t="shared" si="41"/>
+        <v>n/a</v>
+      </c>
+      <c r="G49" s="63">
+        <f t="shared" si="42"/>
+        <v>1.8714760066562697E-4</v>
+      </c>
+      <c r="H49" s="63">
+        <f t="shared" si="43"/>
+        <v>-7.8046062257750903E-2</v>
+      </c>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="L49" s="63" t="str">
+        <f t="shared" si="44"/>
+        <v>n/a</v>
+      </c>
+      <c r="M49" s="63">
+        <f t="shared" si="38"/>
+        <v>3.8688880536839054E-2</v>
+      </c>
+      <c r="N49" s="63">
+        <f t="shared" si="38"/>
+        <v>-2.3413177038095645E-2</v>
+      </c>
+      <c r="O49" s="63">
+        <f t="shared" si="38"/>
+        <v>2.885853387316395E-2</v>
+      </c>
+      <c r="P49" s="63">
+        <f t="shared" si="38"/>
+        <v>-3.3535259795943073E-2</v>
+      </c>
+      <c r="Q49" s="63">
+        <f t="shared" si="38"/>
+        <v>1.7631386311102171E-2</v>
+      </c>
+      <c r="R49" s="63">
+        <f t="shared" si="38"/>
+        <v>7.9870173052551952E-3</v>
+      </c>
+      <c r="S49" s="63">
+        <f t="shared" si="38"/>
+        <v>-1.8769386229742113E-2</v>
+      </c>
+      <c r="T49" s="63">
+        <f t="shared" si="38"/>
+        <v>-4.9586945372707691E-2</v>
+      </c>
+      <c r="U49" s="63">
+        <f t="shared" si="38"/>
+        <v>-2.1786750623926765E-2</v>
+      </c>
+      <c r="V49" s="63">
+        <f t="shared" si="38"/>
+        <v>-9.2913084346182284E-3</v>
+      </c>
+      <c r="W49" s="63">
+        <f t="shared" si="38"/>
+        <v>-1.3942845182056685E-2</v>
+      </c>
+      <c r="X49" s="63">
+        <f>IFERROR(+X41/W41-1,"n/a")</f>
+        <v>-2.9965804598571788E-2</v>
+      </c>
+      <c r="Y49" s="12"/>
+    </row>
+    <row r="50" spans="1:25">
+      <c r="A50" s="33"/>
+      <c r="B50" s="33"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
+      <c r="S50" s="15"/>
+      <c r="T50" s="15"/>
+      <c r="U50" s="15"/>
+      <c r="V50" s="15"/>
+      <c r="W50" s="15"/>
+      <c r="X50" s="15"/>
+      <c r="Y50" s="12"/>
+    </row>
+    <row r="51" spans="1:25">
+      <c r="A51" s="33" t="s">
+        <v>547</v>
+      </c>
+      <c r="B51" s="33"/>
+      <c r="E51" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'is_fy" &amp; F$2 &amp; F$1 &amp; "'!E:E"), INDIRECT("'is_fy" &amp; F$2 &amp; F$1 &amp; "'!A:A"), $A51) / $B$3</f>
+        <v>-79.745999999999995</v>
+      </c>
+      <c r="G51" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'is_fy" &amp; G$2 &amp; G$1 &amp; "'!E:E"), INDIRECT("'is_fy" &amp; G$2 &amp; G$1 &amp; "'!A:A"), $A51) / $B$3</f>
+        <v>-4.2130000000000001</v>
+      </c>
+      <c r="H51" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'is_fy" &amp; H$2 &amp; H$1 &amp; "'!E:E"), INDIRECT("'is_fy" &amp; H$2 &amp; H$1 &amp; "'!A:A"), $A51) / $B$3</f>
+        <v>-557.00800000000004</v>
+      </c>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="L51" s="62">
+        <f t="shared" ref="L51:V51" ca="1" si="45">SUMIFS(INDIRECT("'is_q" &amp; L$2 &amp; L$1 &amp; "'!E:E"), INDIRECT("'is_q" &amp; L$2 &amp; L$1 &amp; "'!A:A"), $A51) / $B$3</f>
+        <v>16.395</v>
+      </c>
+      <c r="M51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>-4.3920000000000003</v>
+      </c>
+      <c r="N51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>18.062999999999999</v>
+      </c>
+      <c r="O51" s="62"/>
+      <c r="P51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>-1.611</v>
+      </c>
+      <c r="Q51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>6.7530000000000001</v>
+      </c>
+      <c r="R51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>16.670999999999999</v>
+      </c>
+      <c r="S51" s="62"/>
+      <c r="T51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>24.617000000000001</v>
+      </c>
+      <c r="U51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>27.395</v>
+      </c>
+      <c r="V51" s="62">
+        <f t="shared" ca="1" si="45"/>
+        <v>-613.19899999999996</v>
+      </c>
+      <c r="W51" s="62"/>
+      <c r="X51" s="62">
+        <f ca="1">SUMIFS(INDIRECT("'is_q" &amp; X$2 &amp; X$1 &amp; "'!E:E"), INDIRECT("'is_q" &amp; X$2 &amp; X$1 &amp; "'!A:A"), $A51) / $B$3</f>
+        <v>13.444000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
+      <c r="A52" s="33"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="11" t="b" cm="1">
+        <f t="array" aca="1" ref="C52" ca="1">AND(F52:AC52&lt;$B$1,F52:AC52&gt;-$B$1)</f>
+        <v>0</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="13">
+        <f ca="1">+F51-F27</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="13">
+        <f ca="1">+G51-G27</f>
+        <v>1.1457501614131615E-13</v>
+      </c>
+      <c r="H52" s="13">
+        <f ca="1">+H51-H27</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="L52" s="34">
+        <f ca="1">+L51-L27</f>
+        <v>1.1690000000000396</v>
+      </c>
+      <c r="M52" s="34">
+        <f ca="1">+M51-M27</f>
+        <v>1.248000000000018</v>
+      </c>
+      <c r="N52" s="34">
+        <f ca="1">+N51-N27</f>
+        <v>0</v>
+      </c>
+      <c r="O52" s="34">
+        <f ca="1">F27-SUM(L27:O27)</f>
+        <v>0</v>
+      </c>
+      <c r="P52" s="34">
+        <f ca="1">+P51-P27</f>
+        <v>1.4432899320127035E-14</v>
+      </c>
+      <c r="Q52" s="34">
+        <f ca="1">+Q51-Q27</f>
+        <v>-2.6645352591003757E-14</v>
+      </c>
+      <c r="R52" s="34">
+        <f ca="1">+R51-R27</f>
+        <v>0</v>
+      </c>
+      <c r="S52" s="34">
+        <f ca="1">G27-SUM(P27:S27)</f>
+        <v>-2.0605739337042905E-13</v>
+      </c>
+      <c r="T52" s="34">
+        <f ca="1">+T51-T27</f>
+        <v>0</v>
+      </c>
+      <c r="U52" s="34">
+        <f ca="1">+U51-U27</f>
+        <v>0</v>
+      </c>
+      <c r="V52" s="34">
+        <f ca="1">+V51-V27</f>
+        <v>0</v>
+      </c>
+      <c r="W52" s="34">
+        <f ca="1">H27-SUM(T27:W27)</f>
+        <v>0</v>
+      </c>
+      <c r="X52" s="34">
+        <f ca="1">+X51-X27</f>
+        <v>2.3092638912203256E-14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
+      <c r="A53" s="33"/>
+      <c r="B53" s="33"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="L53" s="12"/>
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="12"/>
+      <c r="T53" s="12"/>
+      <c r="U53" s="12"/>
+      <c r="V53" s="12"/>
+      <c r="W53" s="12"/>
+      <c r="X53" s="12"/>
+      <c r="Y53" s="12"/>
+    </row>
+    <row r="54" spans="1:25">
+      <c r="A54" s="33"/>
+      <c r="B54" s="33"/>
+      <c r="E54" s="2" t="str">
         <f>Input!$E$8&amp;" - BS"</f>
         <v>BMBL - BS</v>
       </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:41">
-      <c r="A48" s="33"/>
-      <c r="B48" s="33"/>
-      <c r="E48" s="6" t="str">
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:25">
+      <c r="A55" s="33"/>
+      <c r="B55" s="33"/>
+      <c r="E55" s="6" t="str">
         <f>+Input!$E$14</f>
         <v>$mn</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G55" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="H55" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="L48" s="14" t="s">
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="L55" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="M48" s="14" t="s">
+      <c r="M55" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="N48" s="14" t="s">
+      <c r="N55" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="O48" s="14" t="s">
+      <c r="O55" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="P48" s="14" t="s">
+      <c r="P55" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="Q48" s="14" t="s">
+      <c r="Q55" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="R48" s="14" t="s">
+      <c r="R55" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="S48" s="14" t="s">
+      <c r="S55" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="T48" s="14" t="s">
+      <c r="T55" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="U48" s="14" t="s">
+      <c r="U55" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="V48" s="14" t="s">
+      <c r="V55" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="W48" s="14" t="s">
+      <c r="W55" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="X48" s="14" t="s">
+      <c r="X55" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="3" customHeight="1">
-      <c r="A49" s="33"/>
-      <c r="B49" s="33"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-    </row>
-    <row r="50" spans="1:24" s="49" customFormat="1">
-      <c r="A50" s="47" t="s">
+    <row r="56" spans="1:25" ht="3" customHeight="1">
+      <c r="A56" s="33"/>
+      <c r="B56" s="33"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+    </row>
+    <row r="57" spans="1:25" s="49" customFormat="1">
+      <c r="A57" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="48"/>
-      <c r="E50" s="49" t="s">
+      <c r="B57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="E57" s="49" t="s">
         <v>564</v>
       </c>
-      <c r="F50" s="50">
+      <c r="F57" s="50">
         <f>+bs_fy22!C16/B3</f>
         <v>402.55900000000003</v>
       </c>
-      <c r="G50" s="50">
-        <f t="shared" ref="G50:H53" ca="1" si="37">SUMIFS(INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!B:B"), $A50) / $B$3</f>
+      <c r="G57" s="50">
+        <f t="shared" ref="G57:H60" ca="1" si="46">SUMIFS(INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!B:B"), $A57) / $B$3</f>
         <v>355.642</v>
       </c>
-      <c r="H50" s="50">
-        <f t="shared" ca="1" si="37"/>
+      <c r="H57" s="50">
+        <f t="shared" ca="1" si="46"/>
         <v>204.31899999999999</v>
       </c>
-      <c r="I50" s="51"/>
-      <c r="J50" s="51"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="50">
-        <f t="shared" ref="L50:R53" ca="1" si="38">SUMIFS(INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!B:B"), $A50) / $B$3</f>
+      <c r="I57" s="51"/>
+      <c r="J57" s="51"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="50">
+        <f t="shared" ref="L57:R60" ca="1" si="47">SUMIFS(INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!B:B"), $A57) / $B$3</f>
         <v>308.78800000000001</v>
       </c>
-      <c r="M50" s="50">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A50) / $B$3</f>
+      <c r="M57" s="50">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A57) / $B$3</f>
         <v>334.64499999999998</v>
       </c>
-      <c r="N50" s="50">
-        <f t="shared" ca="1" si="38"/>
+      <c r="N57" s="50">
+        <f t="shared" ca="1" si="47"/>
         <v>365.10500000000002</v>
       </c>
-      <c r="O50" s="50">
-        <f>F50</f>
+      <c r="O57" s="50">
+        <f>F57</f>
         <v>402.55900000000003</v>
       </c>
-      <c r="P50" s="50">
-        <f t="shared" ca="1" si="38"/>
+      <c r="P57" s="50">
+        <f t="shared" ca="1" si="47"/>
         <v>388.95499999999998</v>
       </c>
-      <c r="Q50" s="50">
-        <f t="shared" ca="1" si="38"/>
+      <c r="Q57" s="50">
+        <f t="shared" ca="1" si="47"/>
         <v>381.01900000000001</v>
       </c>
-      <c r="R50" s="50">
-        <f t="shared" ca="1" si="38"/>
+      <c r="R57" s="50">
+        <f t="shared" ca="1" si="47"/>
         <v>439.18400000000003</v>
       </c>
-      <c r="S50" s="50">
-        <f ca="1">+G50</f>
+      <c r="S57" s="50">
+        <f ca="1">+G57</f>
         <v>355.642</v>
       </c>
-      <c r="T50" s="50">
-        <f t="shared" ref="T50:V53" ca="1" si="39">SUMIFS(INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!B:B"), $A50) / $B$3</f>
+      <c r="T57" s="50">
+        <f t="shared" ref="T57:V60" ca="1" si="48">SUMIFS(INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!B:B"), $A57) / $B$3</f>
         <v>262.69900000000001</v>
       </c>
-      <c r="U50" s="50">
-        <f t="shared" ca="1" si="39"/>
+      <c r="U57" s="50">
+        <f t="shared" ca="1" si="48"/>
         <v>286.66399999999999</v>
       </c>
-      <c r="V50" s="50">
-        <f t="shared" ca="1" si="39"/>
+      <c r="V57" s="50">
+        <f t="shared" ca="1" si="48"/>
         <v>252.05699999999999</v>
       </c>
-      <c r="W50" s="50">
-        <f ca="1">H50</f>
+      <c r="W57" s="50">
+        <f ca="1">H57</f>
         <v>204.31899999999999</v>
       </c>
-      <c r="X50" s="50">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A50) / $B$3</f>
+      <c r="X57" s="50">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A57) / $B$3</f>
         <v>202.24299999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
-      <c r="A51" s="33" t="s">
+    <row r="58" spans="1:25">
+      <c r="A58" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="33"/>
-      <c r="E51" s="2" t="s">
+      <c r="B58" s="33"/>
+      <c r="E58" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F51" s="38">
+      <c r="F58" s="38">
         <f>+bs_fy22!C26/B3</f>
         <v>3692.6210000000001</v>
       </c>
-      <c r="G51" s="38">
-        <f t="shared" ca="1" si="37"/>
+      <c r="G58" s="38">
+        <f t="shared" ca="1" si="46"/>
         <v>3625.127</v>
       </c>
-      <c r="H51" s="38">
-        <f t="shared" ca="1" si="37"/>
+      <c r="H58" s="38">
+        <f t="shared" ca="1" si="46"/>
         <v>2524.8870000000002</v>
       </c>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="38">
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="39"/>
+      <c r="L58" s="38">
         <f>+bs_q122!C28/B3</f>
         <v>3795.402</v>
       </c>
-      <c r="M51" s="38">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A51) / $B$3</f>
+      <c r="M58" s="38">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A58) / $B$3</f>
         <v>3767.819</v>
       </c>
-      <c r="N51" s="38">
+      <c r="N58" s="38">
         <f>+bs_q322!C28/B3</f>
         <v>3792.8380000000002</v>
       </c>
-      <c r="O51" s="38">
-        <f>F51</f>
+      <c r="O58" s="38">
+        <f>F58</f>
         <v>3692.6210000000001</v>
       </c>
-      <c r="P51" s="38">
-        <f t="shared" ca="1" si="38"/>
+      <c r="P58" s="38">
+        <f t="shared" ca="1" si="47"/>
         <v>3702.5920000000001</v>
       </c>
-      <c r="Q51" s="38">
-        <f t="shared" ca="1" si="38"/>
+      <c r="Q58" s="38">
+        <f t="shared" ca="1" si="47"/>
         <v>3692.297</v>
       </c>
-      <c r="R51" s="38">
-        <f t="shared" ca="1" si="38"/>
+      <c r="R58" s="38">
+        <f t="shared" ca="1" si="47"/>
         <v>3733.1930000000002</v>
       </c>
-      <c r="S51" s="38">
-        <f ca="1">+G51</f>
+      <c r="S58" s="38">
+        <f ca="1">+G58</f>
         <v>3625.127</v>
       </c>
-      <c r="T51" s="38">
-        <f t="shared" ca="1" si="39"/>
+      <c r="T58" s="38">
+        <f t="shared" ca="1" si="48"/>
         <v>3516.9490000000001</v>
       </c>
-      <c r="U51" s="38">
-        <f t="shared" ca="1" si="39"/>
+      <c r="U58" s="38">
+        <f t="shared" ca="1" si="48"/>
         <v>3524.24</v>
       </c>
-      <c r="V51" s="38">
-        <f t="shared" ca="1" si="39"/>
+      <c r="V58" s="38">
+        <f t="shared" ca="1" si="48"/>
         <v>2589.4119999999998</v>
       </c>
-      <c r="W51" s="38">
-        <f ca="1">H51</f>
+      <c r="W58" s="38">
+        <f ca="1">H58</f>
         <v>2524.8870000000002</v>
       </c>
-      <c r="X51" s="38">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A51) / $B$3</f>
+      <c r="X58" s="38">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A58) / $B$3</f>
         <v>2508.2919999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
-      <c r="A52" s="33" t="s">
+    <row r="59" spans="1:25">
+      <c r="A59" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="E52" s="9" t="s">
+      <c r="B59" s="33"/>
+      <c r="E59" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F52" s="39">
+      <c r="F59" s="39">
         <f>+bs_fy22!C55/B3</f>
         <v>1627.8150000000001</v>
       </c>
-      <c r="G52" s="39">
-        <f t="shared" ca="1" si="37"/>
+      <c r="G59" s="39">
+        <f t="shared" ca="1" si="46"/>
         <v>1635.0150000000001</v>
       </c>
-      <c r="H52" s="39">
-        <f t="shared" ca="1" si="37"/>
+      <c r="H59" s="39">
+        <f t="shared" ca="1" si="46"/>
         <v>824.53499999999997</v>
       </c>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39">
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="39"/>
+      <c r="L59" s="39">
         <f>+bs_q122!C61/B3</f>
         <v>1643.2070000000001</v>
       </c>
-      <c r="M52" s="39">
+      <c r="M59" s="39">
         <f>+bs_q222!C61/B3</f>
         <v>1656.027</v>
       </c>
-      <c r="N52" s="39">
+      <c r="N59" s="39">
         <f>+bs_q322!C62/B3</f>
         <v>1695.481</v>
       </c>
-      <c r="O52" s="39">
-        <f>F52</f>
+      <c r="O59" s="39">
+        <f>F59</f>
         <v>1627.8150000000001</v>
       </c>
-      <c r="P52" s="39">
-        <f t="shared" ca="1" si="38"/>
+      <c r="P59" s="39">
+        <f t="shared" ca="1" si="47"/>
         <v>1724.2070000000001</v>
       </c>
-      <c r="Q52" s="39">
-        <f t="shared" ca="1" si="38"/>
+      <c r="Q59" s="39">
+        <f t="shared" ca="1" si="47"/>
         <v>1665.3040000000001</v>
       </c>
-      <c r="R52" s="39">
-        <f t="shared" ca="1" si="38"/>
+      <c r="R59" s="39">
+        <f t="shared" ca="1" si="47"/>
         <v>1689.723</v>
       </c>
-      <c r="S52" s="39">
-        <f ca="1">+G52</f>
+      <c r="S59" s="39">
+        <f ca="1">+G59</f>
         <v>1635.0150000000001</v>
       </c>
-      <c r="T52" s="39">
-        <f t="shared" ca="1" si="39"/>
+      <c r="T59" s="39">
+        <f t="shared" ca="1" si="48"/>
         <v>1604.345</v>
       </c>
-      <c r="U52" s="39">
-        <f t="shared" ca="1" si="39"/>
+      <c r="U59" s="39">
+        <f t="shared" ca="1" si="48"/>
         <v>1652.9269999999999</v>
       </c>
-      <c r="V52" s="39">
-        <f t="shared" ca="1" si="39"/>
+      <c r="V59" s="39">
+        <f t="shared" ca="1" si="48"/>
         <v>852.56200000000001</v>
       </c>
-      <c r="W52" s="39">
-        <f ca="1">H52</f>
+      <c r="W59" s="39">
+        <f ca="1">H59</f>
         <v>824.53499999999997</v>
       </c>
-      <c r="X52" s="39">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A52) / $B$3</f>
+      <c r="X59" s="39">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A59) / $B$3</f>
         <v>814.51400000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
-      <c r="A53" s="33" t="s">
+    <row r="60" spans="1:25">
+      <c r="A60" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="E53" s="9" t="s">
+      <c r="B60" s="33"/>
+      <c r="E60" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F53" s="39">
-        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!B:B"), $A53) / $B$3</f>
+      <c r="F60" s="39">
+        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!B:B"), $A60) / $B$3</f>
         <v>825.76400000000001</v>
       </c>
-      <c r="G53" s="39">
-        <f t="shared" ca="1" si="37"/>
+      <c r="G60" s="39">
+        <f t="shared" ca="1" si="46"/>
         <v>702.25800000000004</v>
       </c>
-      <c r="H53" s="39">
-        <f t="shared" ca="1" si="37"/>
+      <c r="H60" s="39">
+        <f t="shared" ca="1" si="46"/>
         <v>524.51900000000001</v>
       </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39">
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39">
         <f>+bs_q122!C62/B3</f>
         <v>865.93799999999999</v>
       </c>
-      <c r="M53" s="39">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A53) / $B$3</f>
+      <c r="M60" s="39">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A60) / $B$3</f>
         <v>860.48699999999997</v>
       </c>
-      <c r="N53" s="39">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!B:B"), $A53) / $B$3</f>
+      <c r="N60" s="39">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!B:B"), $A60) / $B$3</f>
         <v>866.82299999999998</v>
       </c>
-      <c r="O53" s="39">
-        <f ca="1">F53</f>
+      <c r="O60" s="39">
+        <f ca="1">F60</f>
         <v>825.76400000000001</v>
       </c>
-      <c r="P53" s="39">
-        <f t="shared" ca="1" si="38"/>
+      <c r="P60" s="39">
+        <f t="shared" ca="1" si="47"/>
         <v>712.48900000000003</v>
       </c>
-      <c r="Q53" s="39">
-        <f t="shared" ca="1" si="38"/>
+      <c r="Q60" s="39">
+        <f t="shared" ca="1" si="47"/>
         <v>781.02800000000002</v>
       </c>
-      <c r="R53" s="39">
-        <f t="shared" ca="1" si="38"/>
+      <c r="R60" s="39">
+        <f t="shared" ca="1" si="47"/>
         <v>790.43600000000004</v>
       </c>
-      <c r="S53" s="39">
-        <f ca="1">+G53</f>
+      <c r="S60" s="39">
+        <f ca="1">+G60</f>
         <v>702.25800000000004</v>
       </c>
-      <c r="T53" s="39">
-        <f t="shared" ca="1" si="39"/>
+      <c r="T60" s="39">
+        <f t="shared" ca="1" si="48"/>
         <v>658.85199999999998</v>
       </c>
-      <c r="U53" s="39">
-        <f t="shared" ca="1" si="39"/>
+      <c r="U60" s="39">
+        <f t="shared" ca="1" si="48"/>
         <v>645.07100000000003</v>
       </c>
-      <c r="V53" s="39">
-        <f t="shared" ca="1" si="39"/>
+      <c r="V60" s="39">
+        <f t="shared" ca="1" si="48"/>
         <v>514.30100000000004</v>
       </c>
-      <c r="W53" s="39">
-        <f ca="1">H53</f>
+      <c r="W60" s="39">
+        <f ca="1">H60</f>
         <v>524.51900000000001</v>
       </c>
-      <c r="X53" s="39">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A53) / $B$3</f>
+      <c r="X60" s="39">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A60) / $B$3</f>
         <v>539.72699999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
-      <c r="E54" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F54" s="38">
-        <f ca="1">SUM(F52:F53)</f>
-        <v>2453.5790000000002</v>
-      </c>
-      <c r="G54" s="38">
-        <f ca="1">SUM(G52:G53)</f>
-        <v>2337.2730000000001</v>
-      </c>
-      <c r="H54" s="38">
-        <f ca="1">SUM(H52:H53)</f>
-        <v>1349.0540000000001</v>
-      </c>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="38">
-        <f t="shared" ref="L54:X54" si="40">SUM(L52:L53)</f>
-        <v>2509.145</v>
-      </c>
-      <c r="M54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2516.5140000000001</v>
-      </c>
-      <c r="N54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2562.3040000000001</v>
-      </c>
-      <c r="O54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2453.5790000000002</v>
-      </c>
-      <c r="P54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2436.6959999999999</v>
-      </c>
-      <c r="Q54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2446.3320000000003</v>
-      </c>
-      <c r="R54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2480.1590000000001</v>
-      </c>
-      <c r="S54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2337.2730000000001</v>
-      </c>
-      <c r="T54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2263.1970000000001</v>
-      </c>
-      <c r="U54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>2297.998</v>
-      </c>
-      <c r="V54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>1366.8630000000001</v>
-      </c>
-      <c r="W54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>1349.0540000000001</v>
-      </c>
-      <c r="X54" s="38">
-        <f t="shared" ca="1" si="40"/>
-        <v>1354.241</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24">
-      <c r="A55" s="33"/>
-      <c r="B55" s="33"/>
-      <c r="E55" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" s="38">
-        <f ca="1">+F51-F54</f>
-        <v>1239.0419999999999</v>
-      </c>
-      <c r="G55" s="38">
-        <f ca="1">+G51-G54</f>
-        <v>1287.8539999999998</v>
-      </c>
-      <c r="H55" s="38">
-        <f ca="1">+H51-H54</f>
-        <v>1175.8330000000001</v>
-      </c>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="38">
-        <f t="shared" ref="L55:X55" si="41">+L51-L54</f>
-        <v>1286.2570000000001</v>
-      </c>
-      <c r="M55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1251.3049999999998</v>
-      </c>
-      <c r="N55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1230.5340000000001</v>
-      </c>
-      <c r="O55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1239.0419999999999</v>
-      </c>
-      <c r="P55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1265.8960000000002</v>
-      </c>
-      <c r="Q55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1245.9649999999997</v>
-      </c>
-      <c r="R55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1253.0340000000001</v>
-      </c>
-      <c r="S55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1287.8539999999998</v>
-      </c>
-      <c r="T55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1253.752</v>
-      </c>
-      <c r="U55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1226.2419999999997</v>
-      </c>
-      <c r="V55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1222.5489999999998</v>
-      </c>
-      <c r="W55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1175.8330000000001</v>
-      </c>
-      <c r="X55" s="38">
-        <f t="shared" ca="1" si="41"/>
-        <v>1154.0509999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24">
-      <c r="A56" s="33"/>
-      <c r="B56" s="33"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="12"/>
-      <c r="V56" s="12"/>
-      <c r="W56" s="12"/>
-      <c r="X56" s="12"/>
-    </row>
-    <row r="57" spans="1:24">
-      <c r="A57" s="33"/>
-      <c r="B57" s="33"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="12"/>
-      <c r="S57" s="12"/>
-      <c r="T57" s="12"/>
-      <c r="U57" s="12"/>
-      <c r="V57" s="12"/>
-      <c r="W57" s="12"/>
-      <c r="X57" s="12"/>
-    </row>
-    <row r="58" spans="1:24">
-      <c r="A58" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" s="33"/>
-      <c r="E58" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1239.0419999999999</v>
-      </c>
-      <c r="G58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1287.854</v>
-      </c>
-      <c r="H58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; H$2 &amp; H$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; H$2 &amp; H$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1175.8330000000001</v>
-      </c>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
-      <c r="L58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1286.2570000000001</v>
-      </c>
-      <c r="M58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1251.3050000000001</v>
-      </c>
-      <c r="N58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1230.5340000000001</v>
-      </c>
-      <c r="O58" s="13"/>
-      <c r="P58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; P$2 &amp; P$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; P$2 &amp; P$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1265.896</v>
-      </c>
-      <c r="Q58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; Q$2 &amp; Q$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; Q$2 &amp; Q$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1245.9649999999999</v>
-      </c>
-      <c r="R58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; R$2 &amp; R$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; R$2 &amp; R$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1253.0340000000001</v>
-      </c>
-      <c r="S58" s="13"/>
-      <c r="T58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1253.752</v>
-      </c>
-      <c r="U58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; U$2 &amp; U$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; U$2 &amp; U$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1226.242</v>
-      </c>
-      <c r="V58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; V$2 &amp; V$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; V$2 &amp; V$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1222.549</v>
-      </c>
-      <c r="W58" s="13"/>
-      <c r="X58" s="13">
-        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A58) / $B$3</f>
-        <v>1154.0509999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24">
-      <c r="A59" s="33"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="11" t="b" cm="1">
-        <f t="array" aca="1" ref="C59" ca="1">AND(F59:AC59&lt;$B$1,F59:AC59&gt;-$B$1)</f>
-        <v>1</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F59" s="13">
-        <f ca="1">+F55-F58</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="13">
-        <f ca="1">+G55-G58</f>
-        <v>0</v>
-      </c>
-      <c r="H59" s="13">
-        <f ca="1">+H55-H58</f>
-        <v>0</v>
-      </c>
-      <c r="I59" s="12"/>
-      <c r="J59" s="12"/>
-      <c r="L59" s="13">
-        <f ca="1">+L55-L58</f>
-        <v>0</v>
-      </c>
-      <c r="M59" s="13">
-        <f ca="1">+M55-M58</f>
-        <v>0</v>
-      </c>
-      <c r="N59" s="13">
-        <f ca="1">+N55-N58</f>
-        <v>0</v>
-      </c>
-      <c r="O59" s="13"/>
-      <c r="P59" s="13">
-        <f ca="1">+P55-P58</f>
-        <v>0</v>
-      </c>
-      <c r="Q59" s="13">
-        <f ca="1">+Q55-Q58</f>
-        <v>0</v>
-      </c>
-      <c r="R59" s="13">
-        <f ca="1">+R55-R58</f>
-        <v>0</v>
-      </c>
-      <c r="S59" s="13"/>
-      <c r="T59" s="13">
-        <f ca="1">+T55-T58</f>
-        <v>0</v>
-      </c>
-      <c r="U59" s="13">
-        <f ca="1">+U55-U58</f>
-        <v>0</v>
-      </c>
-      <c r="V59" s="13">
-        <f ca="1">+V55-V58</f>
-        <v>0</v>
-      </c>
-      <c r="W59" s="13"/>
-      <c r="X59" s="13">
-        <f ca="1">+X55-X58</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24">
-      <c r="A60" s="33"/>
-      <c r="B60" s="33"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="L60" s="12"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
-      <c r="P60" s="12"/>
-      <c r="Q60" s="12"/>
-      <c r="R60" s="12"/>
-      <c r="S60" s="12"/>
-      <c r="T60" s="12"/>
-      <c r="U60" s="12"/>
-      <c r="V60" s="12"/>
-      <c r="W60" s="12"/>
-      <c r="X60" s="12"/>
-    </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:25">
       <c r="A61" s="33"/>
       <c r="B61" s="33"/>
-      <c r="E61" s="2" t="str">
+      <c r="E61" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F61" s="38">
+        <f ca="1">SUM(F59:F60)</f>
+        <v>2453.5790000000002</v>
+      </c>
+      <c r="G61" s="38">
+        <f ca="1">SUM(G59:G60)</f>
+        <v>2337.2730000000001</v>
+      </c>
+      <c r="H61" s="38">
+        <f ca="1">SUM(H59:H60)</f>
+        <v>1349.0540000000001</v>
+      </c>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="39"/>
+      <c r="L61" s="38">
+        <f t="shared" ref="L61:X61" si="49">SUM(L59:L60)</f>
+        <v>2509.145</v>
+      </c>
+      <c r="M61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2516.5140000000001</v>
+      </c>
+      <c r="N61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2562.3040000000001</v>
+      </c>
+      <c r="O61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2453.5790000000002</v>
+      </c>
+      <c r="P61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2436.6959999999999</v>
+      </c>
+      <c r="Q61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2446.3320000000003</v>
+      </c>
+      <c r="R61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2480.1590000000001</v>
+      </c>
+      <c r="S61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2337.2730000000001</v>
+      </c>
+      <c r="T61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2263.1970000000001</v>
+      </c>
+      <c r="U61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>2297.998</v>
+      </c>
+      <c r="V61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>1366.8630000000001</v>
+      </c>
+      <c r="W61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>1349.0540000000001</v>
+      </c>
+      <c r="X61" s="38">
+        <f t="shared" ca="1" si="49"/>
+        <v>1354.241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
+      <c r="A62" s="33"/>
+      <c r="B62" s="33"/>
+      <c r="E62" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" s="38">
+        <f ca="1">+F58-F61</f>
+        <v>1239.0419999999999</v>
+      </c>
+      <c r="G62" s="38">
+        <f ca="1">+G58-G61</f>
+        <v>1287.8539999999998</v>
+      </c>
+      <c r="H62" s="38">
+        <f ca="1">+H58-H61</f>
+        <v>1175.8330000000001</v>
+      </c>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="39"/>
+      <c r="L62" s="38">
+        <f t="shared" ref="L62:X62" si="50">+L58-L61</f>
+        <v>1286.2570000000001</v>
+      </c>
+      <c r="M62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1251.3049999999998</v>
+      </c>
+      <c r="N62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1230.5340000000001</v>
+      </c>
+      <c r="O62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1239.0419999999999</v>
+      </c>
+      <c r="P62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1265.8960000000002</v>
+      </c>
+      <c r="Q62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1245.9649999999997</v>
+      </c>
+      <c r="R62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1253.0340000000001</v>
+      </c>
+      <c r="S62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1287.8539999999998</v>
+      </c>
+      <c r="T62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1253.752</v>
+      </c>
+      <c r="U62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1226.2419999999997</v>
+      </c>
+      <c r="V62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1222.5489999999998</v>
+      </c>
+      <c r="W62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1175.8330000000001</v>
+      </c>
+      <c r="X62" s="38">
+        <f t="shared" ca="1" si="50"/>
+        <v>1154.0509999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
+      <c r="A63" s="33"/>
+      <c r="B63" s="33"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="L63" s="12"/>
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+      <c r="O63" s="12"/>
+      <c r="P63" s="12"/>
+      <c r="Q63" s="12"/>
+      <c r="R63" s="12"/>
+      <c r="S63" s="12"/>
+      <c r="T63" s="12"/>
+      <c r="U63" s="12"/>
+      <c r="V63" s="12"/>
+      <c r="W63" s="12"/>
+      <c r="X63" s="12"/>
+    </row>
+    <row r="64" spans="1:25">
+      <c r="A64" s="33"/>
+      <c r="B64" s="33"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="L64" s="12"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="12"/>
+      <c r="O64" s="12"/>
+      <c r="P64" s="12"/>
+      <c r="Q64" s="12"/>
+      <c r="R64" s="12"/>
+      <c r="S64" s="12"/>
+      <c r="T64" s="12"/>
+      <c r="U64" s="12"/>
+      <c r="V64" s="12"/>
+      <c r="W64" s="12"/>
+      <c r="X64" s="12"/>
+    </row>
+    <row r="65" spans="1:31">
+      <c r="A65" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B65" s="33"/>
+      <c r="E65" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; F$2 &amp; F$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1239.0419999999999</v>
+      </c>
+      <c r="G65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; G$2 &amp; G$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1287.854</v>
+      </c>
+      <c r="H65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_fy" &amp; H$2 &amp; H$1 &amp; "'!C:C"), INDIRECT("'bs_fy" &amp; H$2 &amp; H$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1175.8330000000001</v>
+      </c>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="L65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; L$2 &amp; L$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1286.2570000000001</v>
+      </c>
+      <c r="M65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; M$2 &amp; M$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1251.3050000000001</v>
+      </c>
+      <c r="N65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; N$2 &amp; N$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1230.5340000000001</v>
+      </c>
+      <c r="O65" s="13"/>
+      <c r="P65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; P$2 &amp; P$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; P$2 &amp; P$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1265.896</v>
+      </c>
+      <c r="Q65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; Q$2 &amp; Q$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; Q$2 &amp; Q$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1245.9649999999999</v>
+      </c>
+      <c r="R65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; R$2 &amp; R$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; R$2 &amp; R$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1253.0340000000001</v>
+      </c>
+      <c r="S65" s="13"/>
+      <c r="T65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; T$2 &amp; T$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1253.752</v>
+      </c>
+      <c r="U65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; U$2 &amp; U$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; U$2 &amp; U$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1226.242</v>
+      </c>
+      <c r="V65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; V$2 &amp; V$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; V$2 &amp; V$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1222.549</v>
+      </c>
+      <c r="W65" s="13"/>
+      <c r="X65" s="13">
+        <f ca="1">SUMIFS(INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!C:C"), INDIRECT("'bs_q" &amp; X$2 &amp; X$1 &amp; "'!B:B"), $A65) / $B$3</f>
+        <v>1154.0509999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31">
+      <c r="A66" s="33"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="11" t="b" cm="1">
+        <f t="array" aca="1" ref="C66" ca="1">AND(F66:AC66&lt;$B$1,F66:AC66&gt;-$B$1)</f>
+        <v>1</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F66" s="13">
+        <f ca="1">+F62-F65</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="13">
+        <f ca="1">+G62-G65</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="13">
+        <f ca="1">+H62-H65</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="L66" s="13">
+        <f ca="1">+L62-L65</f>
+        <v>0</v>
+      </c>
+      <c r="M66" s="13">
+        <f ca="1">+M62-M65</f>
+        <v>0</v>
+      </c>
+      <c r="N66" s="13">
+        <f ca="1">+N62-N65</f>
+        <v>0</v>
+      </c>
+      <c r="O66" s="13"/>
+      <c r="P66" s="13">
+        <f ca="1">+P62-P65</f>
+        <v>0</v>
+      </c>
+      <c r="Q66" s="13">
+        <f ca="1">+Q62-Q65</f>
+        <v>0</v>
+      </c>
+      <c r="R66" s="13">
+        <f ca="1">+R62-R65</f>
+        <v>0</v>
+      </c>
+      <c r="S66" s="13"/>
+      <c r="T66" s="13">
+        <f ca="1">+T62-T65</f>
+        <v>0</v>
+      </c>
+      <c r="U66" s="13">
+        <f ca="1">+U62-U65</f>
+        <v>0</v>
+      </c>
+      <c r="V66" s="13">
+        <f ca="1">+V62-V65</f>
+        <v>0</v>
+      </c>
+      <c r="W66" s="13"/>
+      <c r="X66" s="13">
+        <f ca="1">+X62-X65</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:31">
+      <c r="A67" s="33"/>
+      <c r="B67" s="33"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="L67" s="12"/>
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+      <c r="O67" s="12"/>
+      <c r="P67" s="12"/>
+      <c r="Q67" s="12"/>
+      <c r="R67" s="12"/>
+      <c r="S67" s="12"/>
+      <c r="T67" s="12"/>
+      <c r="U67" s="12"/>
+      <c r="V67" s="12"/>
+      <c r="W67" s="12"/>
+      <c r="X67" s="12"/>
+    </row>
+    <row r="68" spans="1:31">
+      <c r="A68" s="33"/>
+      <c r="B68" s="33"/>
+      <c r="E68" s="2" t="str">
         <f>Input!$E$8&amp;" - CF"</f>
         <v>BMBL - CF</v>
       </c>
-      <c r="H61" s="5"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
-      <c r="O61" s="19" t="s">
+      <c r="H68" s="5"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="O68" s="19" t="s">
         <v>549</v>
       </c>
-      <c r="P61" s="19"/>
-      <c r="Q61" s="19"/>
-      <c r="R61" s="19"/>
-      <c r="S61" s="19" t="s">
+      <c r="P68" s="19"/>
+      <c r="Q68" s="19"/>
+      <c r="R68" s="19"/>
+      <c r="S68" s="19" t="s">
         <v>549</v>
       </c>
-      <c r="T61" s="19"/>
-      <c r="U61" s="19"/>
-      <c r="V61" s="19"/>
-      <c r="W61" s="19" t="s">
+      <c r="T68" s="19"/>
+      <c r="U68" s="19"/>
+      <c r="V68" s="19"/>
+      <c r="W68" s="19" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
-      <c r="E62" s="6" t="str">
+    <row r="69" spans="1:31">
+      <c r="E69" s="6" t="str">
         <f>+Input!$E$14</f>
         <v>$mn</v>
       </c>
-      <c r="F62" s="14" t="s">
+      <c r="F69" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G62" s="14" t="s">
+      <c r="G69" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="H62" s="14" t="s">
+      <c r="H69" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="I62" s="12"/>
-      <c r="J62" s="12"/>
-      <c r="L62" s="14" t="str">
-        <f t="shared" ref="L62:O62" si="42">L48</f>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="L69" s="14" t="str">
+        <f t="shared" ref="L69:O69" si="51">L55</f>
         <v>Mar 22</v>
       </c>
-      <c r="M62" s="14" t="str">
-        <f t="shared" si="42"/>
+      <c r="M69" s="14" t="str">
+        <f t="shared" si="51"/>
         <v>Jun 22</v>
       </c>
-      <c r="N62" s="14" t="str">
-        <f t="shared" si="42"/>
+      <c r="N69" s="14" t="str">
+        <f t="shared" si="51"/>
         <v>Sep 22</v>
       </c>
-      <c r="O62" s="14" t="str">
-        <f t="shared" si="42"/>
+      <c r="O69" s="14" t="str">
+        <f t="shared" si="51"/>
         <v>Dec 22</v>
       </c>
-      <c r="P62" s="14" t="str">
-        <f t="shared" ref="P62" si="43">P48</f>
+      <c r="P69" s="14" t="str">
+        <f t="shared" ref="P69" si="52">P55</f>
         <v>Mar 23</v>
       </c>
-      <c r="Q62" s="14" t="str">
-        <f t="shared" ref="Q62:S62" si="44">Q48</f>
+      <c r="Q69" s="14" t="str">
+        <f t="shared" ref="Q69:S69" si="53">Q55</f>
         <v>Jun 23</v>
       </c>
-      <c r="R62" s="14" t="str">
-        <f t="shared" si="44"/>
+      <c r="R69" s="14" t="str">
+        <f t="shared" si="53"/>
         <v>Sep 23</v>
       </c>
-      <c r="S62" s="14" t="str">
-        <f t="shared" si="44"/>
+      <c r="S69" s="14" t="str">
+        <f t="shared" si="53"/>
         <v>Dec 23</v>
       </c>
-      <c r="T62" s="14" t="str">
-        <f>T48</f>
+      <c r="T69" s="14" t="str">
+        <f>T55</f>
         <v>Mar 24</v>
       </c>
-      <c r="U62" s="14" t="str">
-        <f t="shared" ref="U62:X62" si="45">U48</f>
+      <c r="U69" s="14" t="str">
+        <f t="shared" ref="U69:X69" si="54">U55</f>
         <v>Jun 24</v>
       </c>
-      <c r="V62" s="14" t="str">
-        <f t="shared" si="45"/>
+      <c r="V69" s="14" t="str">
+        <f t="shared" si="54"/>
         <v>Sep 24</v>
       </c>
-      <c r="W62" s="14" t="str">
-        <f t="shared" si="45"/>
+      <c r="W69" s="14" t="str">
+        <f t="shared" si="54"/>
         <v>Dec 24</v>
       </c>
-      <c r="X62" s="14" t="str">
-        <f t="shared" si="45"/>
+      <c r="X69" s="14" t="str">
+        <f t="shared" si="54"/>
         <v>Mar 25</v>
       </c>
     </row>
-    <row r="63" spans="1:24" ht="3" customHeight="1">
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-    </row>
-    <row r="64" spans="1:24">
-      <c r="B64" s="33"/>
-      <c r="E64" s="9" t="s">
+    <row r="70" spans="1:31" ht="3" customHeight="1">
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+    </row>
+    <row r="71" spans="1:31">
+      <c r="B71" s="33"/>
+      <c r="E71" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F64" s="39">
+      <c r="F71" s="39">
         <f>+cf_fy24!E44/$B$3</f>
         <v>132.941</v>
       </c>
-      <c r="G64" s="39">
+      <c r="G71" s="39">
         <f>+cf_fy24!D44/$B$3</f>
         <v>182.08600000000001</v>
       </c>
-      <c r="H64" s="39">
+      <c r="H71" s="39">
         <f>+cf_fy24!C44/$B$3</f>
         <v>123.441</v>
       </c>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39">
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="39"/>
+      <c r="L71" s="39">
         <f>+cf_q123!D42/$B$3</f>
         <v>19.358000000000001</v>
       </c>
-      <c r="M64" s="39">
-        <f>+cf_q222!C41/$B$3-L64</f>
+      <c r="M71" s="39">
+        <f>+cf_q222!C41/$B$3-L71</f>
         <v>25.409000000000002</v>
       </c>
-      <c r="N64" s="39">
-        <f>+cf_q322!D44/$B$3-SUM(L64:M64)</f>
+      <c r="N71" s="39">
+        <f>+cf_q322!D44/$B$3-SUM(L71:M71)</f>
         <v>37.002000000000002</v>
       </c>
-      <c r="O64" s="39">
-        <f>F64-SUM(L64:N64)</f>
+      <c r="O71" s="39">
+        <f>F71-SUM(L71:N71)</f>
         <v>51.171999999999997</v>
       </c>
-      <c r="P64" s="39">
+      <c r="P71" s="39">
         <f>+cf_q123!C42/$B$3</f>
         <v>13.388999999999999</v>
       </c>
-      <c r="Q64" s="39">
-        <f>+cf_q224!D43/$B$3-P64</f>
+      <c r="Q71" s="39">
+        <f>+cf_q224!D43/$B$3-P71</f>
         <v>42.710999999999999</v>
       </c>
-      <c r="R64" s="39">
-        <f>+cf_q324!E44/$B$3-Q64-P64</f>
+      <c r="R71" s="39">
+        <f>+cf_q324!E44/$B$3-Q71-P71</f>
         <v>62.569000000000003</v>
       </c>
-      <c r="S64" s="39">
-        <f>G64-SUM(P64:R64)</f>
+      <c r="S71" s="39">
+        <f>G71-SUM(P71:R71)</f>
         <v>63.417000000000016</v>
       </c>
-      <c r="T64" s="39">
+      <c r="T71" s="39">
         <f>+cf_q125!D43/$B$3</f>
         <v>2.42</v>
       </c>
-      <c r="U64" s="39">
-        <f>+cf_q224!C43/$B$3-T64</f>
+      <c r="U71" s="39">
+        <f>+cf_q224!C43/$B$3-T71</f>
         <v>32.924999999999997</v>
       </c>
-      <c r="V64" s="39">
-        <f>+cf_q324!C44/$B$3-U64-T64</f>
+      <c r="V71" s="39">
+        <f>+cf_q324!C44/$B$3-U71-T71</f>
         <v>93.494</v>
       </c>
-      <c r="W64" s="39">
-        <f>H64-SUM(T64:V64)</f>
+      <c r="W71" s="39">
+        <f>H71-SUM(T71:V71)</f>
         <v>-5.3979999999999961</v>
       </c>
-      <c r="X64" s="39">
+      <c r="X71" s="39">
         <f>+cf_q125!C43/$B$3</f>
         <v>43.244999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:33">
-      <c r="B65" s="33"/>
-      <c r="E65" s="9" t="s">
+    <row r="72" spans="1:31">
+      <c r="B72" s="33"/>
+      <c r="E72" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F65" s="41">
+      <c r="F72" s="41">
         <f>+cf_fy24!E49/$B$3</f>
         <v>-86.052999999999997</v>
       </c>
-      <c r="G65" s="41">
+      <c r="G72" s="41">
         <f>+cf_fy24!D49/$B$3</f>
         <v>-24.754999999999999</v>
       </c>
-      <c r="H65" s="41">
+      <c r="H72" s="41">
         <f>+cf_fy24!C49/$B$3</f>
         <v>-26.754000000000001</v>
       </c>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="39"/>
-      <c r="L65" s="41">
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="39"/>
+      <c r="L72" s="41">
         <f>+cf_q123!D46/$B$3</f>
         <v>-74.715999999999994</v>
       </c>
-      <c r="M65" s="41">
-        <f>+cf_q222!C46/$B$3-L65</f>
+      <c r="M72" s="41">
+        <f>+cf_q222!C46/$B$3-L72</f>
         <v>-3.0530000000000115</v>
       </c>
-      <c r="N65" s="41">
-        <f>+cf_q322!D49/$B$3-L65-M65</f>
+      <c r="N72" s="41">
+        <f>+cf_q322!D49/$B$3-L72-M72</f>
         <v>-3.2620000000000005</v>
       </c>
-      <c r="O65" s="41">
-        <f>F65-SUM(L65:N65)</f>
+      <c r="O72" s="41">
+        <f>F72-SUM(L72:N72)</f>
         <v>-5.0219999999999914</v>
       </c>
-      <c r="P65" s="41">
+      <c r="P72" s="41">
         <f>+cf_q123!C46/$B$3</f>
         <v>-6.8109999999999999</v>
       </c>
-      <c r="Q65" s="41">
-        <f>+cf_q224!D47/$B$3-P65</f>
+      <c r="Q72" s="41">
+        <f>+cf_q224!D47/$B$3-P72</f>
         <v>-12.276</v>
       </c>
-      <c r="R65" s="41">
-        <f>+cf_q324!E49/$B$3-P65-Q65</f>
+      <c r="R72" s="41">
+        <f>+cf_q324!E49/$B$3-P72-Q72</f>
         <v>-3.5019999999999989</v>
       </c>
-      <c r="S65" s="41">
-        <f>G65-SUM(P65:R65)</f>
+      <c r="S72" s="41">
+        <f>G72-SUM(P72:R72)</f>
         <v>-2.1660000000000004</v>
       </c>
-      <c r="T65" s="41">
+      <c r="T72" s="41">
         <f>+cf_q125!D46/$B$3</f>
         <v>-2.8010000000000002</v>
       </c>
-      <c r="U65" s="41">
-        <f>+cf_q224!C47/$B$3-T65</f>
+      <c r="U72" s="41">
+        <f>+cf_q224!C47/$B$3-T72</f>
         <v>-1.7299999999999995</v>
       </c>
-      <c r="V65" s="41">
-        <f>+cf_q324!C49/$B$3-T65-U65</f>
+      <c r="V72" s="41">
+        <f>+cf_q324!C49/$B$3-T72-U72</f>
         <v>-19.053999999999998</v>
       </c>
-      <c r="W65" s="41">
-        <f>H65-SUM(T65:V65)</f>
+      <c r="W72" s="41">
+        <f>H72-SUM(T72:V72)</f>
         <v>-3.169000000000004</v>
       </c>
-      <c r="X65" s="41">
+      <c r="X72" s="41">
         <f>+cf_q125!C46/$B$3</f>
         <v>-2.411</v>
       </c>
     </row>
-    <row r="66" spans="1:33">
-      <c r="B66" s="33"/>
-      <c r="E66" s="2" t="s">
+    <row r="73" spans="1:31">
+      <c r="B73" s="33"/>
+      <c r="E73" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F66" s="38">
-        <f>+F64+F65</f>
+      <c r="F73" s="38">
+        <f>+F71+F72</f>
         <v>46.888000000000005</v>
       </c>
-      <c r="G66" s="38">
-        <f>+G64+G65</f>
+      <c r="G73" s="38">
+        <f>+G71+G72</f>
         <v>157.33100000000002</v>
       </c>
-      <c r="H66" s="38">
-        <f>+H64+H65</f>
+      <c r="H73" s="38">
+        <f>+H71+H72</f>
         <v>96.686999999999998</v>
       </c>
-      <c r="I66" s="38"/>
-      <c r="J66" s="38"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="38">
-        <f t="shared" ref="L66:R66" si="46">+L64+L65</f>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="39"/>
+      <c r="L73" s="38">
+        <f t="shared" ref="L73:R73" si="55">+L71+L72</f>
         <v>-55.35799999999999</v>
       </c>
-      <c r="M66" s="38">
-        <f t="shared" si="46"/>
+      <c r="M73" s="38">
+        <f t="shared" si="55"/>
         <v>22.355999999999991</v>
       </c>
-      <c r="N66" s="38">
-        <f t="shared" si="46"/>
+      <c r="N73" s="38">
+        <f t="shared" si="55"/>
         <v>33.74</v>
       </c>
-      <c r="O66" s="38">
-        <f t="shared" si="46"/>
+      <c r="O73" s="38">
+        <f t="shared" si="55"/>
         <v>46.150000000000006</v>
       </c>
-      <c r="P66" s="38">
-        <f t="shared" si="46"/>
+      <c r="P73" s="38">
+        <f t="shared" si="55"/>
         <v>6.5779999999999994</v>
       </c>
-      <c r="Q66" s="38">
-        <f t="shared" si="46"/>
+      <c r="Q73" s="38">
+        <f t="shared" si="55"/>
         <v>30.434999999999999</v>
       </c>
-      <c r="R66" s="38">
-        <f t="shared" si="46"/>
+      <c r="R73" s="38">
+        <f t="shared" si="55"/>
         <v>59.067000000000007</v>
       </c>
-      <c r="S66" s="38">
-        <f t="shared" ref="S66:S68" si="47">G66-SUM(P66:R66)</f>
+      <c r="S73" s="38">
+        <f t="shared" ref="S73:S75" si="56">G73-SUM(P73:R73)</f>
         <v>61.251000000000005</v>
       </c>
-      <c r="T66" s="38">
-        <f>+T64+T65</f>
+      <c r="T73" s="38">
+        <f>+T71+T72</f>
         <v>-0.38100000000000023</v>
       </c>
-      <c r="U66" s="38">
-        <f>+U64+U65</f>
+      <c r="U73" s="38">
+        <f>+U71+U72</f>
         <v>31.194999999999997</v>
       </c>
-      <c r="V66" s="38">
-        <f>+V64+V65</f>
+      <c r="V73" s="38">
+        <f>+V71+V72</f>
         <v>74.44</v>
       </c>
-      <c r="W66" s="38">
-        <f t="shared" ref="W66:W68" si="48">H66-SUM(T66:V66)</f>
+      <c r="W73" s="38">
+        <f t="shared" ref="W73:W75" si="57">H73-SUM(T73:V73)</f>
         <v>-8.5669999999999931</v>
       </c>
-      <c r="X66" s="38">
-        <f>+X64+X65</f>
+      <c r="X73" s="38">
+        <f>+X71+X72</f>
         <v>40.833999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
-      <c r="A67" s="33"/>
-      <c r="B67" s="33"/>
-      <c r="E67" s="9" t="s">
+    <row r="74" spans="1:31">
+      <c r="A74" s="33"/>
+      <c r="B74" s="33"/>
+      <c r="E74" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F67" s="39">
+      <c r="F74" s="39">
         <f>+cf_fy24!E60/$B$3</f>
         <v>-14.954000000000001</v>
       </c>
-      <c r="G67" s="39">
+      <c r="G74" s="39">
         <f>+cf_fy24!D60/$B$3</f>
         <v>-198.89099999999999</v>
       </c>
-      <c r="H67" s="39">
+      <c r="H74" s="39">
         <f>+cf_fy24!C60/$B$3</f>
         <v>-250.828</v>
       </c>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-      <c r="L67" s="39">
+      <c r="I74" s="39"/>
+      <c r="J74" s="39"/>
+      <c r="K74" s="39"/>
+      <c r="L74" s="39">
         <f>+cf_q123!D53/$B$3</f>
         <v>-7.1459999999999999</v>
       </c>
-      <c r="M67" s="39">
-        <f>+cf_q222!C56/$B$3-L67</f>
+      <c r="M74" s="39">
+        <f>+cf_q222!C56/$B$3-L74</f>
         <v>-1.9230000000000009</v>
       </c>
-      <c r="N67" s="39">
-        <f>+cf_q322!D60/$B$3-M67-L67</f>
+      <c r="N74" s="39">
+        <f>+cf_q322!D60/$B$3-M74-L74</f>
         <v>-2.5959999999999974</v>
       </c>
-      <c r="O67" s="39">
-        <f t="shared" ref="O67:O68" si="49">F67-SUM(L67:N67)</f>
+      <c r="O74" s="39">
+        <f t="shared" ref="O74:O75" si="58">F74-SUM(L74:N74)</f>
         <v>-3.2890000000000015</v>
       </c>
-      <c r="P67" s="39">
+      <c r="P74" s="39">
         <f>+cf_q123!C53/$B$3</f>
         <v>-16.167999999999999</v>
       </c>
-      <c r="Q67" s="39">
-        <f>+cf_q224!D55/$B$3-P67</f>
+      <c r="Q74" s="39">
+        <f>+cf_q224!D55/$B$3-P74</f>
         <v>-38.532000000000004</v>
       </c>
-      <c r="R67" s="39">
-        <f>+cf_q324!E58/$B$3-P67-Q67</f>
+      <c r="R74" s="39">
+        <f>+cf_q324!E58/$B$3-P74-Q74</f>
         <v>-3.654999999999994</v>
       </c>
-      <c r="S67" s="39">
-        <f t="shared" si="47"/>
+      <c r="S74" s="39">
+        <f t="shared" si="56"/>
         <v>-140.536</v>
       </c>
-      <c r="T67" s="39">
+      <c r="T74" s="39">
         <f>+cf_q125!D55/$B$3</f>
         <v>-94.366</v>
       </c>
-      <c r="U67" s="39">
-        <f>+cf_q224!C55/$B$3-T67</f>
+      <c r="U74" s="39">
+        <f>+cf_q224!C55/$B$3-T74</f>
         <v>-6.6370000000000005</v>
       </c>
-      <c r="V67" s="39">
-        <f>+cf_q324!C58/$B$3-T67-U67</f>
+      <c r="V74" s="39">
+        <f>+cf_q324!C58/$B$3-T74-U74</f>
         <v>-106.746</v>
       </c>
-      <c r="W67" s="39">
-        <f t="shared" si="48"/>
+      <c r="W74" s="39">
+        <f t="shared" si="57"/>
         <v>-43.079000000000008</v>
       </c>
-      <c r="X67" s="39">
+      <c r="X74" s="39">
         <f>+cf_q125!C55/$B$3</f>
         <v>-42.466000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:33">
-      <c r="A68" s="33"/>
-      <c r="B68" s="33"/>
-      <c r="E68" s="22" t="s">
+    <row r="75" spans="1:31">
+      <c r="A75" s="33"/>
+      <c r="B75" s="33"/>
+      <c r="E75" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F68" s="43">
+      <c r="F75" s="43">
         <f>+cf_fy24!E55/$B$3</f>
         <v>0</v>
       </c>
-      <c r="G68" s="43">
+      <c r="G75" s="43">
         <f>+cf_fy24!D55/$B$3</f>
         <v>-112.83</v>
       </c>
-      <c r="H68" s="43">
+      <c r="H75" s="43">
         <f>+cf_fy24!C55/$B$3</f>
         <v>-192.113</v>
       </c>
-      <c r="I68" s="43"/>
-      <c r="J68" s="43"/>
-      <c r="K68" s="39"/>
-      <c r="L68" s="39">
+      <c r="I75" s="43"/>
+      <c r="J75" s="43"/>
+      <c r="K75" s="39"/>
+      <c r="L75" s="39">
         <v>0</v>
       </c>
-      <c r="M68" s="39">
+      <c r="M75" s="39">
         <v>0</v>
       </c>
-      <c r="N68" s="39">
+      <c r="N75" s="39">
         <v>0</v>
       </c>
-      <c r="O68" s="39">
-        <f t="shared" si="49"/>
+      <c r="O75" s="39">
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
-      <c r="P68" s="39">
+      <c r="P75" s="39">
         <v>0</v>
       </c>
-      <c r="Q68" s="39">
-        <f>+cf_q224!D51/$B$3-P68</f>
+      <c r="Q75" s="39">
+        <f>+cf_q224!D51/$B$3-P75</f>
         <v>-20.89</v>
       </c>
-      <c r="R68" s="39">
-        <f>+cf_q324!E53/$B$3-Q68-P68</f>
+      <c r="R75" s="39">
+        <f>+cf_q324!E53/$B$3-Q75-P75</f>
         <v>0</v>
       </c>
-      <c r="S68" s="39">
-        <f t="shared" si="47"/>
+      <c r="S75" s="39">
+        <f t="shared" si="56"/>
         <v>-91.94</v>
       </c>
-      <c r="T68" s="39">
+      <c r="T75" s="39">
         <f>+cf_q125!D50/$B$3</f>
         <v>-62.107999999999997</v>
       </c>
-      <c r="U68" s="39">
-        <f>+cf_q224!C51/$B$3-T68</f>
+      <c r="U75" s="39">
+        <f>+cf_q224!C51/$B$3-T75</f>
         <v>0</v>
       </c>
-      <c r="V68" s="39">
-        <f>+cf_q324!C53/$B$3-T68-U68</f>
+      <c r="V75" s="39">
+        <f>+cf_q324!C53/$B$3-T75-U75</f>
         <v>-89.734999999999985</v>
       </c>
-      <c r="W68" s="39">
-        <f t="shared" si="48"/>
+      <c r="W75" s="39">
+        <f t="shared" si="57"/>
         <v>-40.27000000000001</v>
       </c>
-      <c r="X68" s="39">
+      <c r="X75" s="39">
         <f>+cf_q125!C50/$B$3</f>
         <v>-28.681999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:33">
-      <c r="X69" s="39">
-        <f>X68/6</f>
+    <row r="76" spans="1:31">
+      <c r="X76" s="39">
+        <f>X75/6</f>
         <v>-4.7803333333333331</v>
       </c>
     </row>
-    <row r="70" spans="1:33">
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="12"/>
-      <c r="I70" s="12"/>
-      <c r="J70" s="12"/>
-      <c r="L70" s="12"/>
-      <c r="M70" s="12"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="12"/>
-      <c r="P70" s="12"/>
-      <c r="Q70" s="12"/>
-      <c r="R70" s="12"/>
-      <c r="S70" s="12"/>
-      <c r="T70" s="12"/>
-      <c r="U70" s="12"/>
-      <c r="V70" s="12"/>
-      <c r="W70" s="12"/>
-      <c r="X70" s="12"/>
-    </row>
-    <row r="71" spans="1:33">
-      <c r="E71" t="s">
-        <v>72</v>
-      </c>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
-      <c r="H71" s="12"/>
-      <c r="I71" s="12"/>
-      <c r="J71" s="12"/>
-      <c r="L71" s="23"/>
-      <c r="M71" s="23"/>
-      <c r="N71" s="23"/>
-      <c r="O71" s="23"/>
-      <c r="P71" s="23"/>
-      <c r="Q71" s="23"/>
-      <c r="R71" s="23"/>
-      <c r="S71" s="23"/>
-      <c r="T71" s="23"/>
-      <c r="U71" s="23"/>
-      <c r="V71" s="23"/>
-      <c r="W71" s="23"/>
-      <c r="X71" s="56">
-        <v>103.291444</v>
-      </c>
-      <c r="Y71" s="44"/>
-      <c r="Z71" s="44"/>
-      <c r="AA71" s="44"/>
-      <c r="AB71" s="44"/>
-      <c r="AC71" s="44"/>
-      <c r="AD71" s="44"/>
-      <c r="AE71" s="44"/>
-    </row>
-    <row r="72" spans="1:33">
-      <c r="E72" t="s">
-        <v>559</v>
-      </c>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15"/>
-      <c r="L72" s="12"/>
-      <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="12"/>
-      <c r="P72" s="12"/>
-      <c r="Q72" s="12"/>
-      <c r="R72" s="12"/>
-      <c r="S72" s="12"/>
-      <c r="T72" s="12"/>
-      <c r="U72" s="12"/>
-      <c r="V72" s="12"/>
-      <c r="W72" s="12"/>
-      <c r="X72" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="73" spans="1:33">
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
-      <c r="I73" s="12"/>
-      <c r="J73" s="12"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="12"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="12"/>
-      <c r="R73" s="12"/>
-      <c r="S73" s="12"/>
-      <c r="T73" s="12"/>
-      <c r="U73" s="12"/>
-      <c r="V73" s="12"/>
-      <c r="W73" s="12"/>
-      <c r="X73" s="12"/>
-      <c r="Y73" s="12"/>
-      <c r="Z73" s="12"/>
-      <c r="AA73" s="12"/>
-      <c r="AB73" s="12"/>
-      <c r="AC73" s="12"/>
-      <c r="AD73" s="12"/>
-      <c r="AE73" s="12"/>
-    </row>
-    <row r="74" spans="1:33">
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
-      <c r="I74" s="12"/>
-      <c r="J74" s="12"/>
-      <c r="L74" s="12"/>
-      <c r="M74" s="12"/>
-      <c r="N74" s="12"/>
-      <c r="O74" s="12"/>
-      <c r="P74" s="12"/>
-      <c r="Q74" s="12"/>
-      <c r="R74" s="12"/>
-      <c r="S74" s="12"/>
-      <c r="T74" s="12"/>
-      <c r="U74" s="12"/>
-      <c r="V74" s="12"/>
-      <c r="W74" s="12"/>
-      <c r="X74" s="12"/>
-      <c r="Y74" s="12"/>
-    </row>
-    <row r="75" spans="1:33">
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
-      <c r="I75" s="12"/>
-      <c r="J75" s="12"/>
-      <c r="L75" s="12"/>
-      <c r="M75" s="12"/>
-      <c r="N75" s="12"/>
-      <c r="O75" s="12"/>
-      <c r="P75" s="12"/>
-      <c r="Q75" s="12"/>
-      <c r="R75" s="12"/>
-      <c r="S75" s="12"/>
-      <c r="T75" s="12"/>
-      <c r="U75" s="12"/>
-      <c r="V75" s="12"/>
-      <c r="W75" s="12"/>
-      <c r="X75" s="12"/>
-      <c r="Y75" s="12"/>
-    </row>
-    <row r="76" spans="1:33">
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
-      <c r="H76" s="12"/>
-      <c r="I76" s="12"/>
-      <c r="J76" s="12"/>
-      <c r="L76" s="12"/>
-      <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
-      <c r="O76" s="12"/>
-      <c r="P76" s="12"/>
-      <c r="Q76" s="12"/>
-      <c r="R76" s="12"/>
-      <c r="S76" s="12"/>
-      <c r="T76" s="12"/>
-      <c r="U76" s="12"/>
-      <c r="V76" s="12"/>
-      <c r="W76" s="12"/>
-      <c r="X76" s="12"/>
-      <c r="Y76" s="5"/>
-      <c r="Z76" s="5"/>
-      <c r="AA76" s="5"/>
-      <c r="AB76" s="5"/>
-      <c r="AC76" s="5"/>
-      <c r="AD76" s="5"/>
-      <c r="AE76" s="5"/>
-      <c r="AF76" s="5"/>
-      <c r="AG76" s="5"/>
-    </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:31">
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
       <c r="H77" s="12"/>
@@ -21443,89 +21746,48 @@
       <c r="V77" s="12"/>
       <c r="W77" s="12"/>
       <c r="X77" s="12"/>
-      <c r="Y77" s="36" t="s">
-        <v>550</v>
-      </c>
-      <c r="Z77" s="36" t="s">
-        <v>551</v>
-      </c>
-      <c r="AA77" s="36" t="s">
-        <v>552</v>
-      </c>
-      <c r="AB77" s="36" t="s">
-        <v>553</v>
-      </c>
-      <c r="AC77" s="36" t="s">
-        <v>554</v>
-      </c>
-      <c r="AD77" s="36" t="s">
-        <v>555</v>
-      </c>
-      <c r="AE77" s="36" t="s">
-        <v>556</v>
-      </c>
-      <c r="AF77" s="36" t="s">
-        <v>553</v>
-      </c>
-      <c r="AG77" s="36" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="78" spans="1:33">
+    </row>
+    <row r="78" spans="1:31">
+      <c r="E78" t="s">
+        <v>72</v>
+      </c>
       <c r="F78" s="12"/>
       <c r="G78" s="12"/>
       <c r="H78" s="12"/>
       <c r="I78" s="12"/>
       <c r="J78" s="12"/>
-      <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="12"/>
-      <c r="P78" s="12"/>
-      <c r="Q78" s="12"/>
-      <c r="R78" s="12"/>
-      <c r="S78" s="12"/>
-      <c r="T78" s="12"/>
-      <c r="U78" s="12"/>
-      <c r="V78" s="12"/>
-      <c r="W78" s="12"/>
-      <c r="X78" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y78" s="53">
-        <v>243</v>
-      </c>
-      <c r="Z78" s="53">
-        <v>240</v>
-      </c>
-      <c r="AA78" s="53">
-        <v>233</v>
-      </c>
-      <c r="AB78" s="53">
-        <v>226</v>
-      </c>
-      <c r="AC78" s="53">
-        <v>224</v>
-      </c>
-      <c r="AD78" s="53">
-        <v>225</v>
-      </c>
-      <c r="AE78" s="53">
-        <v>226</v>
-      </c>
-      <c r="AF78" s="53">
-        <v>225</v>
-      </c>
-      <c r="AG78" s="53">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="79" spans="1:33">
+      <c r="L78" s="23"/>
+      <c r="M78" s="23"/>
+      <c r="N78" s="23"/>
+      <c r="O78" s="23"/>
+      <c r="P78" s="23"/>
+      <c r="Q78" s="23"/>
+      <c r="R78" s="23"/>
+      <c r="S78" s="23"/>
+      <c r="T78" s="23"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="23"/>
+      <c r="W78" s="23"/>
+      <c r="X78" s="56">
+        <v>103.291444</v>
+      </c>
+      <c r="Y78" s="44"/>
+      <c r="Z78" s="44"/>
+      <c r="AA78" s="44"/>
+      <c r="AB78" s="44"/>
+      <c r="AC78" s="44"/>
+      <c r="AD78" s="44"/>
+      <c r="AE78" s="44"/>
+    </row>
+    <row r="79" spans="1:31">
+      <c r="E79" t="s">
+        <v>559</v>
+      </c>
       <c r="F79" s="12"/>
       <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12"/>
       <c r="N79" s="12"/>
@@ -21538,38 +21800,11 @@
       <c r="U79" s="12"/>
       <c r="V79" s="12"/>
       <c r="W79" s="12"/>
-      <c r="X79" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y79" s="53">
-        <v>85.32</v>
-      </c>
-      <c r="Z79" s="53">
-        <v>75.78</v>
-      </c>
-      <c r="AA79" s="53">
-        <v>70.62</v>
-      </c>
-      <c r="AB79" s="53">
-        <v>63.9</v>
-      </c>
-      <c r="AC79" s="53">
-        <v>67.28</v>
-      </c>
-      <c r="AD79" s="53">
-        <v>69.739999999999995</v>
-      </c>
-      <c r="AE79" s="53">
-        <v>68.010000000000005</v>
-      </c>
-      <c r="AF79" s="53">
-        <v>72.989999999999995</v>
-      </c>
-      <c r="AG79" s="53">
-        <v>71.849999999999994</v>
-      </c>
-    </row>
-    <row r="80" spans="1:33" ht="13.5" thickBot="1">
+      <c r="X79" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:31">
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
@@ -21587,36 +21822,14 @@
       <c r="U80" s="12"/>
       <c r="V80" s="12"/>
       <c r="W80" s="12"/>
-      <c r="X80" s="12" t="s">
-        <v>547</v>
-      </c>
-      <c r="Y80" s="54">
-        <v>41.68</v>
-      </c>
-      <c r="Z80" s="54">
-        <v>30.75</v>
-      </c>
-      <c r="AA80" s="54">
-        <v>22.6</v>
-      </c>
-      <c r="AB80" s="54">
-        <v>22.61</v>
-      </c>
-      <c r="AC80" s="54">
-        <v>14.14</v>
-      </c>
-      <c r="AD80" s="54">
-        <v>38.39</v>
-      </c>
-      <c r="AE80" s="54">
-        <v>26.95</v>
-      </c>
-      <c r="AF80" s="54">
-        <v>21.27</v>
-      </c>
-      <c r="AG80" s="54">
-        <v>16.39</v>
-      </c>
+      <c r="X80" s="12"/>
+      <c r="Y80" s="12"/>
+      <c r="Z80" s="12"/>
+      <c r="AA80" s="12"/>
+      <c r="AB80" s="12"/>
+      <c r="AC80" s="12"/>
+      <c r="AD80" s="12"/>
+      <c r="AE80" s="12"/>
     </row>
     <row r="81" spans="6:33">
       <c r="F81" s="12"/>
@@ -21637,15 +21850,7 @@
       <c r="V81" s="12"/>
       <c r="W81" s="12"/>
       <c r="X81" s="12"/>
-      <c r="Y81" s="55"/>
-      <c r="Z81" s="55"/>
-      <c r="AA81" s="55"/>
-      <c r="AB81" s="55"/>
-      <c r="AC81" s="55"/>
-      <c r="AD81" s="55"/>
-      <c r="AE81" s="55"/>
-      <c r="AF81" s="55"/>
-      <c r="AG81" s="55"/>
+      <c r="Y81" s="12"/>
     </row>
     <row r="82" spans="6:33">
       <c r="F82" s="12"/>
@@ -21665,32 +21870,8 @@
       <c r="U82" s="12"/>
       <c r="V82" s="12"/>
       <c r="W82" s="12"/>
-      <c r="X82" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="Y82" s="55">
-        <v>0.34</v>
-      </c>
-      <c r="Z82" s="55">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="AA82" s="55">
-        <v>0.23</v>
-      </c>
-      <c r="AB82" s="55">
-        <v>0.2</v>
-      </c>
-      <c r="AC82" s="55">
-        <v>0.21</v>
-      </c>
-      <c r="AD82" s="55">
-        <v>0.33</v>
-      </c>
-      <c r="AE82" s="55">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="AF82" s="55"/>
-      <c r="AG82" s="55"/>
+      <c r="X82" s="12"/>
+      <c r="Y82" s="12"/>
     </row>
     <row r="83" spans="6:33">
       <c r="F83" s="12"/>
@@ -21711,7 +21892,15 @@
       <c r="V83" s="12"/>
       <c r="W83" s="12"/>
       <c r="X83" s="12"/>
-      <c r="Y83" s="12"/>
+      <c r="Y83" s="5"/>
+      <c r="Z83" s="5"/>
+      <c r="AA83" s="5"/>
+      <c r="AB83" s="5"/>
+      <c r="AC83" s="5"/>
+      <c r="AD83" s="5"/>
+      <c r="AE83" s="5"/>
+      <c r="AF83" s="5"/>
+      <c r="AG83" s="5"/>
     </row>
     <row r="84" spans="6:33">
       <c r="F84" s="12"/>
@@ -21732,7 +21921,33 @@
       <c r="V84" s="12"/>
       <c r="W84" s="12"/>
       <c r="X84" s="12"/>
-      <c r="Y84" s="12"/>
+      <c r="Y84" s="36" t="s">
+        <v>550</v>
+      </c>
+      <c r="Z84" s="36" t="s">
+        <v>551</v>
+      </c>
+      <c r="AA84" s="36" t="s">
+        <v>552</v>
+      </c>
+      <c r="AB84" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="AC84" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="AD84" s="36" t="s">
+        <v>555</v>
+      </c>
+      <c r="AE84" s="36" t="s">
+        <v>556</v>
+      </c>
+      <c r="AF84" s="36" t="s">
+        <v>553</v>
+      </c>
+      <c r="AG84" s="36" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="85" spans="6:33">
       <c r="F85" s="12"/>
@@ -21752,8 +21967,36 @@
       <c r="U85" s="12"/>
       <c r="V85" s="12"/>
       <c r="W85" s="12"/>
-      <c r="X85" s="12"/>
-      <c r="Y85" s="12"/>
+      <c r="X85" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y85" s="53">
+        <v>243</v>
+      </c>
+      <c r="Z85" s="53">
+        <v>240</v>
+      </c>
+      <c r="AA85" s="53">
+        <v>233</v>
+      </c>
+      <c r="AB85" s="53">
+        <v>226</v>
+      </c>
+      <c r="AC85" s="53">
+        <v>224</v>
+      </c>
+      <c r="AD85" s="53">
+        <v>225</v>
+      </c>
+      <c r="AE85" s="53">
+        <v>226</v>
+      </c>
+      <c r="AF85" s="53">
+        <v>225</v>
+      </c>
+      <c r="AG85" s="53">
+        <v>231</v>
+      </c>
     </row>
     <row r="86" spans="6:33">
       <c r="F86" s="12"/>
@@ -21773,10 +22016,38 @@
       <c r="U86" s="12"/>
       <c r="V86" s="12"/>
       <c r="W86" s="12"/>
-      <c r="X86" s="12"/>
-      <c r="Y86" s="12"/>
-    </row>
-    <row r="87" spans="6:33">
+      <c r="X86" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y86" s="53">
+        <v>85.32</v>
+      </c>
+      <c r="Z86" s="53">
+        <v>75.78</v>
+      </c>
+      <c r="AA86" s="53">
+        <v>70.62</v>
+      </c>
+      <c r="AB86" s="53">
+        <v>63.9</v>
+      </c>
+      <c r="AC86" s="53">
+        <v>67.28</v>
+      </c>
+      <c r="AD86" s="53">
+        <v>69.739999999999995</v>
+      </c>
+      <c r="AE86" s="53">
+        <v>68.010000000000005</v>
+      </c>
+      <c r="AF86" s="53">
+        <v>72.989999999999995</v>
+      </c>
+      <c r="AG86" s="53">
+        <v>71.849999999999994</v>
+      </c>
+    </row>
+    <row r="87" spans="6:33" ht="13.5" thickBot="1">
       <c r="F87" s="12"/>
       <c r="G87" s="12"/>
       <c r="H87" s="12"/>
@@ -21794,8 +22065,36 @@
       <c r="U87" s="12"/>
       <c r="V87" s="12"/>
       <c r="W87" s="12"/>
-      <c r="X87" s="12"/>
-      <c r="Y87" s="12"/>
+      <c r="X87" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="Y87" s="54">
+        <v>41.68</v>
+      </c>
+      <c r="Z87" s="54">
+        <v>30.75</v>
+      </c>
+      <c r="AA87" s="54">
+        <v>22.6</v>
+      </c>
+      <c r="AB87" s="54">
+        <v>22.61</v>
+      </c>
+      <c r="AC87" s="54">
+        <v>14.14</v>
+      </c>
+      <c r="AD87" s="54">
+        <v>38.39</v>
+      </c>
+      <c r="AE87" s="54">
+        <v>26.95</v>
+      </c>
+      <c r="AF87" s="54">
+        <v>21.27</v>
+      </c>
+      <c r="AG87" s="54">
+        <v>16.39</v>
+      </c>
     </row>
     <row r="88" spans="6:33">
       <c r="F88" s="12"/>
@@ -21816,7 +22115,15 @@
       <c r="V88" s="12"/>
       <c r="W88" s="12"/>
       <c r="X88" s="12"/>
-      <c r="Y88" s="12"/>
+      <c r="Y88" s="55"/>
+      <c r="Z88" s="55"/>
+      <c r="AA88" s="55"/>
+      <c r="AB88" s="55"/>
+      <c r="AC88" s="55"/>
+      <c r="AD88" s="55"/>
+      <c r="AE88" s="55"/>
+      <c r="AF88" s="55"/>
+      <c r="AG88" s="55"/>
     </row>
     <row r="89" spans="6:33">
       <c r="F89" s="12"/>
@@ -21836,8 +22143,32 @@
       <c r="U89" s="12"/>
       <c r="V89" s="12"/>
       <c r="W89" s="12"/>
-      <c r="X89" s="12"/>
-      <c r="Y89" s="12"/>
+      <c r="X89" s="12" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y89" s="55">
+        <v>0.34</v>
+      </c>
+      <c r="Z89" s="55">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA89" s="55">
+        <v>0.23</v>
+      </c>
+      <c r="AB89" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="AC89" s="55">
+        <v>0.21</v>
+      </c>
+      <c r="AD89" s="55">
+        <v>0.33</v>
+      </c>
+      <c r="AE89" s="55">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AF89" s="55"/>
+      <c r="AG89" s="55"/>
     </row>
     <row r="90" spans="6:33">
       <c r="F90" s="12"/>
@@ -35573,18 +35904,165 @@
       <c r="X743" s="12"/>
       <c r="Y743" s="12"/>
     </row>
+    <row r="744" spans="6:25">
+      <c r="F744" s="12"/>
+      <c r="G744" s="12"/>
+      <c r="H744" s="12"/>
+      <c r="I744" s="12"/>
+      <c r="J744" s="12"/>
+      <c r="L744" s="12"/>
+      <c r="M744" s="12"/>
+      <c r="N744" s="12"/>
+      <c r="O744" s="12"/>
+      <c r="P744" s="12"/>
+      <c r="Q744" s="12"/>
+      <c r="R744" s="12"/>
+      <c r="S744" s="12"/>
+      <c r="T744" s="12"/>
+      <c r="U744" s="12"/>
+      <c r="V744" s="12"/>
+      <c r="W744" s="12"/>
+      <c r="X744" s="12"/>
+      <c r="Y744" s="12"/>
+    </row>
+    <row r="745" spans="6:25">
+      <c r="F745" s="12"/>
+      <c r="G745" s="12"/>
+      <c r="H745" s="12"/>
+      <c r="I745" s="12"/>
+      <c r="J745" s="12"/>
+      <c r="L745" s="12"/>
+      <c r="M745" s="12"/>
+      <c r="N745" s="12"/>
+      <c r="O745" s="12"/>
+      <c r="P745" s="12"/>
+      <c r="Q745" s="12"/>
+      <c r="R745" s="12"/>
+      <c r="S745" s="12"/>
+      <c r="T745" s="12"/>
+      <c r="U745" s="12"/>
+      <c r="V745" s="12"/>
+      <c r="W745" s="12"/>
+      <c r="X745" s="12"/>
+      <c r="Y745" s="12"/>
+    </row>
+    <row r="746" spans="6:25">
+      <c r="F746" s="12"/>
+      <c r="G746" s="12"/>
+      <c r="H746" s="12"/>
+      <c r="I746" s="12"/>
+      <c r="J746" s="12"/>
+      <c r="L746" s="12"/>
+      <c r="M746" s="12"/>
+      <c r="N746" s="12"/>
+      <c r="O746" s="12"/>
+      <c r="P746" s="12"/>
+      <c r="Q746" s="12"/>
+      <c r="R746" s="12"/>
+      <c r="S746" s="12"/>
+      <c r="T746" s="12"/>
+      <c r="U746" s="12"/>
+      <c r="V746" s="12"/>
+      <c r="W746" s="12"/>
+      <c r="X746" s="12"/>
+      <c r="Y746" s="12"/>
+    </row>
+    <row r="747" spans="6:25">
+      <c r="F747" s="12"/>
+      <c r="G747" s="12"/>
+      <c r="H747" s="12"/>
+      <c r="I747" s="12"/>
+      <c r="J747" s="12"/>
+      <c r="L747" s="12"/>
+      <c r="M747" s="12"/>
+      <c r="N747" s="12"/>
+      <c r="O747" s="12"/>
+      <c r="P747" s="12"/>
+      <c r="Q747" s="12"/>
+      <c r="R747" s="12"/>
+      <c r="S747" s="12"/>
+      <c r="T747" s="12"/>
+      <c r="U747" s="12"/>
+      <c r="V747" s="12"/>
+      <c r="W747" s="12"/>
+      <c r="X747" s="12"/>
+      <c r="Y747" s="12"/>
+    </row>
+    <row r="748" spans="6:25">
+      <c r="F748" s="12"/>
+      <c r="G748" s="12"/>
+      <c r="H748" s="12"/>
+      <c r="I748" s="12"/>
+      <c r="J748" s="12"/>
+      <c r="L748" s="12"/>
+      <c r="M748" s="12"/>
+      <c r="N748" s="12"/>
+      <c r="O748" s="12"/>
+      <c r="P748" s="12"/>
+      <c r="Q748" s="12"/>
+      <c r="R748" s="12"/>
+      <c r="S748" s="12"/>
+      <c r="T748" s="12"/>
+      <c r="U748" s="12"/>
+      <c r="V748" s="12"/>
+      <c r="W748" s="12"/>
+      <c r="X748" s="12"/>
+      <c r="Y748" s="12"/>
+    </row>
+    <row r="749" spans="6:25">
+      <c r="F749" s="12"/>
+      <c r="G749" s="12"/>
+      <c r="H749" s="12"/>
+      <c r="I749" s="12"/>
+      <c r="J749" s="12"/>
+      <c r="L749" s="12"/>
+      <c r="M749" s="12"/>
+      <c r="N749" s="12"/>
+      <c r="O749" s="12"/>
+      <c r="P749" s="12"/>
+      <c r="Q749" s="12"/>
+      <c r="R749" s="12"/>
+      <c r="S749" s="12"/>
+      <c r="T749" s="12"/>
+      <c r="U749" s="12"/>
+      <c r="V749" s="12"/>
+      <c r="W749" s="12"/>
+      <c r="X749" s="12"/>
+      <c r="Y749" s="12"/>
+    </row>
+    <row r="750" spans="6:25">
+      <c r="F750" s="12"/>
+      <c r="G750" s="12"/>
+      <c r="H750" s="12"/>
+      <c r="I750" s="12"/>
+      <c r="J750" s="12"/>
+      <c r="L750" s="12"/>
+      <c r="M750" s="12"/>
+      <c r="N750" s="12"/>
+      <c r="O750" s="12"/>
+      <c r="P750" s="12"/>
+      <c r="Q750" s="12"/>
+      <c r="R750" s="12"/>
+      <c r="S750" s="12"/>
+      <c r="T750" s="12"/>
+      <c r="U750" s="12"/>
+      <c r="V750" s="12"/>
+      <c r="W750" s="12"/>
+      <c r="X750" s="12"/>
+      <c r="Y750" s="12"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="C66">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added high level DDM
</commit_message>
<xml_diff>
--- a/BMBL.xlsx
+++ b/BMBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Development\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72EE4CC-7495-4C68-83E8-E69A2D7C0B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEF0559-474B-4508-8B5F-22F9CC4B997E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="946" activeTab="3" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3188" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3189" uniqueCount="576">
   <si>
     <r>
       <t xml:space="preserve">This Excel file is intended </t>
@@ -1865,9 +1865,6 @@
   </si>
   <si>
     <t>30 Jun</t>
-  </si>
-  <si>
-    <t>WACC</t>
   </si>
   <si>
     <t>discount factor</t>
@@ -17180,8 +17177,8 @@
   </sheetPr>
   <dimension ref="A1:AG750"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA44" sqref="AA44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -17407,7 +17404,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="AF9" s="12"/>
+      <c r="AF9" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="AG9" s="12"/>
     </row>
     <row r="10" spans="1:33" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -19604,7 +19603,7 @@
         <v>3.7772000000000001</v>
       </c>
       <c r="Z37" t="s">
-        <v>573</v>
+        <v>29</v>
       </c>
       <c r="AA37" s="15">
         <v>0.1</v>
@@ -19720,7 +19719,7 @@
         <v>26.85</v>
       </c>
       <c r="Z39" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AE39" s="15"/>
       <c r="AF39" s="15">
@@ -19789,7 +19788,7 @@
         <v>11.57</v>
       </c>
       <c r="Z40" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AA40" s="54">
         <f>1/(1+AA37)^AA9</f>
@@ -20020,7 +20019,7 @@
         <v>-7.7019642593413096E-2</v>
       </c>
       <c r="Z43" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AA43" s="38">
         <f ca="1">+SUM(AA41:AF41)</f>

</xml_diff>

<commit_message>
Added DDM and sensitivities
</commit_message>
<xml_diff>
--- a/BMBL.xlsx
+++ b/BMBL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konst\Development\valuations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEF0559-474B-4508-8B5F-22F9CC4B997E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C54D59E-449D-4ED6-B7FF-5A32275615A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="946" activeTab="3" xr2:uid="{A454576F-BA0E-4C95-85A1-1E0F525C6E61}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3189" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3194" uniqueCount="580">
   <si>
     <r>
       <t xml:space="preserve">This Excel file is intended </t>
@@ -1875,6 +1875,18 @@
   <si>
     <t>Fair Value</t>
   </si>
+  <si>
+    <t>Shareprice</t>
+  </si>
+  <si>
+    <t>0 due to impairment</t>
+  </si>
+  <si>
+    <t>Revenue growth rate</t>
+  </si>
+  <si>
+    <t>$BMBL price per share</t>
+  </si>
 </sst>
 </file>
 
@@ -1892,7 +1904,7 @@
     <numFmt numFmtId="171" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="174" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1995,8 +2007,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4" tint="0.79998168889431442"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2024,6 +2050,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2079,7 +2123,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2185,6 +2229,25 @@
     </xf>
     <xf numFmtId="170" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="5" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="16" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="17" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2226,9 +2289,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0066CC"/>
       <color rgb="FF0366CC"/>
       <color rgb="FF009900"/>
-      <color rgb="FF0066CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -17175,10 +17238,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:AG750"/>
+  <dimension ref="A1:AO750"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z38" sqref="Z38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AI41" sqref="AI41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -17190,7 +17253,8 @@
     <col min="8" max="8" width="10.140625" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="2.85546875" customWidth="1" outlineLevel="1"/>
     <col min="10" max="18" width="8.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.28515625" customWidth="1"/>
+    <col min="26" max="26" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" s="4" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -17658,7 +17722,7 @@
       </c>
       <c r="AF13" s="37">
         <f t="shared" si="5"/>
-        <v>1090.75822817472</v>
+        <v>1096.1314214169602</v>
       </c>
       <c r="AG13" s="38"/>
     </row>
@@ -18156,11 +18220,11 @@
         <v>228.34399999999999</v>
       </c>
       <c r="AB19" s="37">
-        <f t="shared" ref="AB19:AF19" si="11">AB13*AB30</f>
+        <f>AB13*AB30</f>
         <v>232.91087999999999</v>
       </c>
       <c r="AC19" s="37">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="AB19:AF19" si="11">AC13*AC30</f>
         <v>237.56909760000002</v>
       </c>
       <c r="AD19" s="37">
@@ -18173,7 +18237,7 @@
       </c>
       <c r="AF19" s="37">
         <f t="shared" si="11"/>
-        <v>250.87439248018561</v>
+        <v>252.11022692590086</v>
       </c>
       <c r="AG19" s="38"/>
     </row>
@@ -18367,7 +18431,7 @@
       </c>
       <c r="AF21" s="39">
         <f ca="1">+AE21*(1+$AF$39)</f>
-        <v>-38.915100000000002</v>
+        <v>-39.106800000000007</v>
       </c>
       <c r="AG21" s="38"/>
     </row>
@@ -18466,7 +18530,7 @@
       </c>
       <c r="AF22" s="37">
         <f t="shared" ca="1" si="15"/>
-        <v>211.95929248018561</v>
+        <v>213.00342692590084</v>
       </c>
       <c r="AG22" s="38"/>
     </row>
@@ -18567,7 +18631,7 @@
       </c>
       <c r="AF23" s="39">
         <f>+AE23*(1+$AF$39)</f>
-        <v>-10.412884999999999</v>
+        <v>-10.464180000000001</v>
       </c>
       <c r="AG23" s="38"/>
     </row>
@@ -18666,7 +18730,7 @@
       </c>
       <c r="AF24" s="37">
         <f t="shared" ca="1" si="23"/>
-        <v>201.54640748018562</v>
+        <v>202.53924692590084</v>
       </c>
       <c r="AG24" s="38"/>
     </row>
@@ -18745,16 +18809,17 @@
       <c r="W25" s="50">
         <v>-6.4690000000000003</v>
       </c>
+      <c r="Z25" t="s">
+        <v>577</v>
+      </c>
       <c r="AA25" s="38">
-        <f ca="1">+AA24*-AA32</f>
-        <v>-44.936250000000001</v>
+        <v>0</v>
       </c>
       <c r="AB25" s="38">
-        <f t="shared" ref="AB25:AF25" ca="1" si="25">+AB24*-AB32</f>
-        <v>-46.077969999999993</v>
+        <v>0</v>
       </c>
       <c r="AC25" s="38">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ref="AC25:AF25" ca="1" si="25">+AC24*-AC32</f>
         <v>-47.242524400000008</v>
       </c>
       <c r="AD25" s="38">
@@ -18767,7 +18832,7 @@
       </c>
       <c r="AF25" s="38">
         <f t="shared" ca="1" si="25"/>
-        <v>-50.386601870046405</v>
+        <v>-50.63481173147521</v>
       </c>
       <c r="AG25" s="38"/>
     </row>
@@ -18868,7 +18933,7 @@
       </c>
       <c r="AF26" s="39">
         <f t="shared" ref="AF26" ca="1" si="28">+AF24*-AF34</f>
-        <v>-40.30928149603713</v>
+        <v>-40.507849385180172</v>
       </c>
       <c r="AG26" s="38"/>
     </row>
@@ -18947,11 +19012,11 @@
       </c>
       <c r="AA27" s="37">
         <f ca="1">SUM(AA24:AA26)</f>
-        <v>98.859749999999991</v>
+        <v>143.79599999999999</v>
       </c>
       <c r="AB27" s="37">
         <f t="shared" ref="AB27:AF27" ca="1" si="35">SUM(AB24:AB26)</f>
-        <v>101.37153399999998</v>
+        <v>147.44950399999999</v>
       </c>
       <c r="AC27" s="37">
         <f t="shared" ca="1" si="35"/>
@@ -18967,7 +19032,7 @@
       </c>
       <c r="AF27" s="37">
         <f t="shared" ca="1" si="35"/>
-        <v>110.85052411410209</v>
+        <v>111.39658580924544</v>
       </c>
       <c r="AG27" s="38"/>
     </row>
@@ -19072,7 +19137,7 @@
       </c>
       <c r="AF29" s="15">
         <f>+AF39</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AG29" s="38"/>
     </row>
@@ -19156,11 +19221,11 @@
         <v>0.23</v>
       </c>
       <c r="AC30" s="15">
-        <f t="shared" ref="AC30:AE30" si="40">+AB30</f>
+        <f>+AB30</f>
         <v>0.23</v>
       </c>
       <c r="AD30" s="15">
-        <f t="shared" si="40"/>
+        <f t="shared" ref="AC30:AE30" si="40">+AC30</f>
         <v>0.23</v>
       </c>
       <c r="AE30" s="15">
@@ -19350,7 +19415,7 @@
       </c>
       <c r="AG32" s="38"/>
     </row>
-    <row r="33" spans="1:33" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:41" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA33" s="38"/>
       <c r="AB33" s="38"/>
       <c r="AC33" s="38"/>
@@ -19359,7 +19424,7 @@
       <c r="AF33" s="38"/>
       <c r="AG33" s="38"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="E34" s="2" t="s">
@@ -19392,7 +19457,7 @@
       </c>
       <c r="AG34" s="38"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A35" s="33"/>
       <c r="B35" s="33"/>
       <c r="E35" s="3" t="s">
@@ -19460,7 +19525,7 @@
       <c r="AF35" s="38"/>
       <c r="AG35" s="38"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A36" s="33"/>
       <c r="B36" s="33"/>
       <c r="E36" s="3" t="s">
@@ -19528,7 +19593,7 @@
       <c r="AF36" s="38"/>
       <c r="AG36" s="38"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A37" s="33"/>
       <c r="B37" s="33"/>
       <c r="E37" s="42" t="s">
@@ -19626,11 +19691,11 @@
       </c>
       <c r="AF37" s="15">
         <f>AE37-AF39</f>
-        <v>8.5000000000000006E-2</v>
+        <v>0.08</v>
       </c>
       <c r="AG37" s="38"/>
     </row>
-    <row r="38" spans="1:33" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:41" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="33"/>
       <c r="B38" s="33"/>
       <c r="F38" s="47"/>
@@ -19658,7 +19723,7 @@
       <c r="AF38" s="38"/>
       <c r="AG38" s="38"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A39" s="33"/>
       <c r="B39" s="33"/>
       <c r="E39" s="3" t="s">
@@ -19723,11 +19788,11 @@
       </c>
       <c r="AE39" s="15"/>
       <c r="AF39" s="15">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AG39" s="38"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A40" s="33"/>
       <c r="B40" s="33"/>
       <c r="E40" s="3" t="s">
@@ -19812,11 +19877,11 @@
       </c>
       <c r="AF40" s="38">
         <f>AE40/AF37</f>
-        <v>7.3049567418724104</v>
+        <v>7.7615165382394364</v>
       </c>
       <c r="AG40" s="38"/>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A41" s="33"/>
       <c r="B41" s="33"/>
       <c r="E41" s="42" t="s">
@@ -19892,11 +19957,11 @@
       </c>
       <c r="AA41" s="38">
         <f ca="1">+AA40*AA27</f>
-        <v>89.872499999999988</v>
+        <v>130.72363636363636</v>
       </c>
       <c r="AB41" s="38">
         <f t="shared" ref="AB41:AF41" ca="1" si="53">+AB40*AB27</f>
-        <v>83.778127272727247</v>
+        <v>121.85909421487601</v>
       </c>
       <c r="AC41" s="38">
         <f t="shared" ca="1" si="53"/>
@@ -19912,11 +19977,11 @@
       </c>
       <c r="AF41" s="38">
         <f t="shared" ca="1" si="53"/>
-        <v>809.75828346740025</v>
+        <v>864.60644306186703</v>
       </c>
       <c r="AG41" s="38"/>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A42" s="33"/>
       <c r="B42" s="33"/>
       <c r="F42" s="12"/>
@@ -19944,7 +20009,7 @@
       <c r="AF42" s="38"/>
       <c r="AG42" s="38"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A43" s="33"/>
       <c r="B43" s="33"/>
       <c r="E43" s="3" t="s">
@@ -20023,10 +20088,10 @@
       </c>
       <c r="AA43" s="38">
         <f ca="1">+SUM(AA41:AF41)</f>
-        <v>1202.080905394263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
+        <v>1335.861168294515</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="E44" s="3" t="s">
@@ -20101,7 +20166,7 @@
         <v>-2.2123555079231361E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="E45" s="42" t="s">
@@ -20175,8 +20240,15 @@
         <f>IFERROR(+W37/V37-1,"n/a")</f>
         <v>-5.9157595835305332E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="Z45" t="s">
+        <v>576</v>
+      </c>
+      <c r="AA45" s="38">
+        <f ca="1">AA43/W78</f>
+        <v>12.850769202744933</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A46" s="33"/>
       <c r="B46" s="33"/>
       <c r="E46" s="3"/>
@@ -20197,8 +20269,11 @@
       <c r="U46" s="12"/>
       <c r="V46" s="12"/>
       <c r="W46" s="12"/>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AI46" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
       <c r="B47" s="33"/>
       <c r="E47" s="3" t="s">
@@ -20272,8 +20347,17 @@
         <f>IFERROR(+W39/V39-1,"n/a")</f>
         <v>8.0917874396135403E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AI47" s="62"/>
+      <c r="AJ47" s="62"/>
+      <c r="AK47" s="56" t="s">
+        <v>578</v>
+      </c>
+      <c r="AL47" s="56"/>
+      <c r="AM47" s="56"/>
+      <c r="AN47" s="56"/>
+      <c r="AO47" s="56"/>
+    </row>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
       <c r="B48" s="33"/>
       <c r="E48" s="3" t="s">
@@ -20347,8 +20431,32 @@
         <f>IFERROR(+W40/V40-1,"n/a")</f>
         <v>7.9291044776119257E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AI48" s="62"/>
+      <c r="AJ48" s="61">
+        <f ca="1">AA45</f>
+        <v>12.850769202744933</v>
+      </c>
+      <c r="AK48" s="57">
+        <f>AL48-0.01</f>
+        <v>0</v>
+      </c>
+      <c r="AL48" s="57">
+        <f>AM48-0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="AM48" s="63">
+        <v>0.02</v>
+      </c>
+      <c r="AN48" s="57">
+        <f>+AM48+0.01</f>
+        <v>0.03</v>
+      </c>
+      <c r="AO48" s="57">
+        <f>+AN48+0.01</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="49" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A49" s="33"/>
       <c r="B49" s="33"/>
       <c r="E49" s="42" t="s">
@@ -20422,8 +20530,31 @@
         <f>IFERROR(+W41/V41-1,"n/a")</f>
         <v>7.0971169899492592E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AI49" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ49" s="57">
+        <f>+AJ50-0.01</f>
+        <v>0.21</v>
+      </c>
+      <c r="AK49" s="59">
+        <f t="dataTable" ref="AK49:AO53" dt2D="1" dtr="1" r1="AB29" r2="AA30" ca="1"/>
+        <v>10.571448171006207</v>
+      </c>
+      <c r="AL49" s="59">
+        <v>11.00659794660103</v>
+      </c>
+      <c r="AM49" s="59">
+        <v>11.45389879415962</v>
+      </c>
+      <c r="AN49" s="59">
+        <v>11.913584652566493</v>
+      </c>
+      <c r="AO49" s="59">
+        <v>12.385891720985244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A50" s="33"/>
       <c r="B50" s="33"/>
       <c r="F50" s="12"/>
@@ -20443,8 +20574,28 @@
       <c r="U50" s="15"/>
       <c r="V50" s="15"/>
       <c r="W50" s="15"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AI50" s="55"/>
+      <c r="AJ50" s="57">
+        <f>+AJ51-0.01</f>
+        <v>0.22</v>
+      </c>
+      <c r="AK50" s="59">
+        <v>11.227861917053463</v>
+      </c>
+      <c r="AL50" s="58">
+        <v>11.683733110533757</v>
+      </c>
+      <c r="AM50" s="58">
+        <v>12.152333998452278</v>
+      </c>
+      <c r="AN50" s="58">
+        <v>12.633909659640427</v>
+      </c>
+      <c r="AO50" s="59">
+        <v>13.128707540841024</v>
+      </c>
+    </row>
+    <row r="51" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A51" s="33" t="s">
         <v>546</v>
       </c>
@@ -20510,8 +20661,27 @@
       <c r="W51" s="51">
         <v>-253.744</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AI51" s="55"/>
+      <c r="AJ51" s="63">
+        <v>0.23</v>
+      </c>
+      <c r="AK51" s="59">
+        <v>11.884275663100722</v>
+      </c>
+      <c r="AL51" s="58">
+        <v>12.360868274466476</v>
+      </c>
+      <c r="AM51" s="60">
+        <v>12.850769202744933</v>
+      </c>
+      <c r="AN51" s="58">
+        <v>13.354234666714365</v>
+      </c>
+      <c r="AO51" s="59">
+        <v>13.871523360696806</v>
+      </c>
+    </row>
+    <row r="52" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A52" s="33"/>
       <c r="B52" s="33"/>
       <c r="C52" s="11" t="b" cm="1">
@@ -20589,8 +20759,28 @@
         <f>+W51-W27</f>
         <v>2.8999999999996362E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AI52" s="55"/>
+      <c r="AJ52" s="57">
+        <f>+AJ51+0.01</f>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="AK52" s="59">
+        <v>12.540689409147976</v>
+      </c>
+      <c r="AL52" s="58">
+        <v>13.038003438399199</v>
+      </c>
+      <c r="AM52" s="58">
+        <v>13.549204407037591</v>
+      </c>
+      <c r="AN52" s="58">
+        <v>14.074559673788302</v>
+      </c>
+      <c r="AO52" s="59">
+        <v>14.614339180552591</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A53" s="33"/>
       <c r="B53" s="33"/>
       <c r="F53" s="12"/>
@@ -20610,8 +20800,28 @@
       <c r="U53" s="12"/>
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AI53" s="55"/>
+      <c r="AJ53" s="57">
+        <f>+AJ52+0.01</f>
+        <v>0.25</v>
+      </c>
+      <c r="AK53" s="59">
+        <v>13.197103155195229</v>
+      </c>
+      <c r="AL53" s="59">
+        <v>13.715138602331923</v>
+      </c>
+      <c r="AM53" s="59">
+        <v>14.247639611330248</v>
+      </c>
+      <c r="AN53" s="59">
+        <v>14.794884680862236</v>
+      </c>
+      <c r="AO53" s="59">
+        <v>15.357155000408367</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A54" s="33"/>
       <c r="B54" s="33"/>
       <c r="E54" s="2" t="str">
@@ -20620,7 +20830,7 @@
       </c>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A55" s="33"/>
       <c r="B55" s="33"/>
       <c r="E55" s="6" t="str">
@@ -20679,11 +20889,11 @@
         <v>570</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:41" ht="3" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="33"/>
       <c r="B56" s="33"/>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A57" s="33" t="s">
         <v>137</v>
       </c>
@@ -20760,7 +20970,7 @@
         <v>261.73899999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A58" s="33" t="s">
         <v>17</v>
       </c>
@@ -20837,7 +21047,7 @@
         <v>2161.4949999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A59" s="33" t="s">
         <v>92</v>
       </c>
@@ -20914,7 +21124,7 @@
         <v>577.61099999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A60" s="33" t="s">
         <v>91</v>
       </c>
@@ -20991,7 +21201,7 @@
         <v>426.88200000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A61" s="33"/>
       <c r="B61" s="33"/>
       <c r="E61" s="10" t="s">
@@ -21067,7 +21277,7 @@
         <v>1004.4929999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A62" s="33"/>
       <c r="B62" s="33"/>
       <c r="E62" s="10" t="s">
@@ -21143,7 +21353,7 @@
         <v>1157.002</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A63" s="33"/>
       <c r="B63" s="33"/>
       <c r="E63" s="9"/>
@@ -21165,7 +21375,7 @@
       <c r="V63" s="12"/>
       <c r="W63" s="12"/>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A64" s="33"/>
       <c r="B64" s="33"/>
       <c r="F64" s="12"/>
@@ -34643,6 +34853,10 @@
       <c r="W750" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AI49:AI53"/>
+    <mergeCell ref="AK47:AO47"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>TRUE</formula>

</xml_diff>